<commit_message>
fixed error in TOPSIS ranking
Fixed issue with ranking of the alternatives in TOPSIS.
</commit_message>
<xml_diff>
--- a/dmsan/data/criteria_weight_scenarios.xlsx
+++ b/dmsan/data/criteria_weight_scenarios.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hlohm\Dropbox\Lohman-Guest_Shared\12_PhD_Paper3_Sanitation_Decision-Making\Python Code\GitHubDesktop\DMsan\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hlohm\Dropbox\Lohman-Guest_Shared\12_PhD_Paper3_Sanitation_Decision-Making\Python Code\GitHubDesktop\DMsan\dmsan\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D72D1A1-A376-4640-B671-D8267D230EA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{501B47DC-C670-45B6-A9D2-D2E688A34866}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="27210" yWindow="1425" windowWidth="19140" windowHeight="10200" xr2:uid="{E854125C-2344-44F6-A254-41B8AFA7B554}"/>
+    <workbookView xWindow="28680" yWindow="-135" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{E854125C-2344-44F6-A254-41B8AFA7B554}"/>
   </bookViews>
   <sheets>
     <sheet name="definitions" sheetId="4" r:id="rId1"/>
@@ -837,8 +837,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DAC3413-5145-4E90-ADD4-96F1E182146D}">
   <dimension ref="A1:H37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2:G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1966,8 +1966,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCC343D5-ACEC-440C-BE2B-40BCC1E75BAA}">
   <dimension ref="A1:AF3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I33" sqref="I33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Updated technology scores and beneficial vs non-beneficial indicator
Updated technology scores based on scores in SI version 3.

Updated end-user disposal and end-user privacy to both be non-beneficial indicators.
</commit_message>
<xml_diff>
--- a/dmsan/data/criteria_weight_scenarios.xlsx
+++ b/dmsan/data/criteria_weight_scenarios.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hlohm\Dropbox\Lohman-Guest_Shared\12_PhD_Paper3_Sanitation_Decision-Making\Python Code\GitHubDesktop\DMsan\dmsan\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{501B47DC-C670-45B6-A9D2-D2E688A34866}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{998CF5A5-6E93-459A-8BEB-866E68F312D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-135" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{E854125C-2344-44F6-A254-41B8AFA7B554}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{E854125C-2344-44F6-A254-41B8AFA7B554}"/>
   </bookViews>
   <sheets>
     <sheet name="definitions" sheetId="4" r:id="rId1"/>
@@ -838,7 +838,7 @@
   <dimension ref="A1:H37"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:G33"/>
+      <selection activeCell="G33" sqref="G2:G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1423,11 +1423,11 @@
         <v>64</v>
       </c>
       <c r="F24" s="15" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G24" s="15">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.35">
@@ -1471,11 +1471,11 @@
         <v>66</v>
       </c>
       <c r="F26" s="15" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G26" s="15">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.35">
@@ -1967,7 +1967,7 @@
   <dimension ref="A1:AF3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I33" sqref="I33"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2236,13 +2236,13 @@
         <v>1</v>
       </c>
       <c r="W3" s="17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X3" s="17">
         <v>1</v>
       </c>
       <c r="Y3" s="17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z3" s="17">
         <v>1</v>

</xml_diff>

<commit_message>
update codes for evaluation using multiple criteria weights, update results
</commit_message>
<xml_diff>
--- a/dmsan/data/criteria_weight_scenarios.xlsx
+++ b/dmsan/data/criteria_weight_scenarios.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/torimorgan/Documents/GitHub/DMsan/dmsan/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bfca01abaf64aab7/Coding/ds/dmsan/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C9980BB-C809-8949-A4CE-551CD5B3F79D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="36360" yWindow="500" windowWidth="23240" windowHeight="21100" activeTab="1" xr2:uid="{E854125C-2344-44F6-A254-41B8AFA7B554}"/>
+    <workbookView xWindow="3700" yWindow="500" windowWidth="35940" windowHeight="19500" activeTab="1" xr2:uid="{E854125C-2344-44F6-A254-41B8AFA7B554}"/>
   </bookViews>
   <sheets>
     <sheet name="definitions" sheetId="4" r:id="rId1"/>
@@ -1916,8 +1916,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6956783-CD8A-4021-B812-DCE07115A14C}">
   <dimension ref="A1:I53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="E53" sqref="E53"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+      <selection activeCell="B51" sqref="B2:B51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
add uncertainties to AHP value, fix previous inconsistency in social tech scores and system simulation scores, use new method for global weight scenarios, make new figures
</commit_message>
<xml_diff>
--- a/dmsan/data/criteria_weight_scenarios.xlsx
+++ b/dmsan/data/criteria_weight_scenarios.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bfca01abaf64aab7/Coding/ds/dmsan/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C9980BB-C809-8949-A4CE-551CD5B3F79D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{4C9980BB-C809-8949-A4CE-551CD5B3F79D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8BAD0884-E2BE-154C-B4CE-7A7EA24F1A5A}"/>
   <bookViews>
-    <workbookView xWindow="3700" yWindow="500" windowWidth="35940" windowHeight="19500" activeTab="1" xr2:uid="{E854125C-2344-44F6-A254-41B8AFA7B554}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="2" xr2:uid="{E854125C-2344-44F6-A254-41B8AFA7B554}"/>
   </bookViews>
   <sheets>
     <sheet name="definitions" sheetId="4" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="230">
   <si>
     <t>LCA</t>
   </si>
@@ -840,11 +840,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -1179,7 +1178,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DAC3413-5145-4E90-ADD4-96F1E182146D}">
   <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView topLeftCell="C6" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G2" sqref="G2:G29"/>
     </sheetView>
   </sheetViews>
@@ -1215,686 +1214,686 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
+    <row r="2" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" s="4" t="s">
+      <c r="D2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="G2" s="4">
+      <c r="G2" s="3">
         <f>IF(F2="beneficial", 1, 0)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
+    <row r="3" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="G3" s="4">
+      <c r="G3" s="3">
         <f t="shared" ref="G3:G29" si="0">IF(F3="beneficial", 1, 0)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="4" t="s">
+    <row r="4" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="F4" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="G4" s="4">
+      <c r="G4" s="3">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="4" t="s">
+    <row r="5" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="F5" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="G5" s="4">
+      <c r="G5" s="3">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="4" t="s">
+    <row r="6" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="F6" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="G6" s="4">
+      <c r="G6" s="3">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="4" t="s">
+    <row r="7" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="E7" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="F7" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="G7" s="4">
+      <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="5" t="s">
+    <row r="8" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="C8" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="12" t="s">
+      <c r="D8" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="E8" s="12" t="s">
+      <c r="E8" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="F8" s="12" t="s">
+      <c r="F8" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="G8" s="12">
+      <c r="G8" s="11">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="5" t="s">
+    <row r="9" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C9" s="12" t="s">
+      <c r="C9" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D9" s="12" t="s">
+      <c r="D9" s="11" t="s">
         <v>102</v>
       </c>
-      <c r="E9" s="12" t="s">
+      <c r="E9" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="F9" s="12" t="s">
+      <c r="F9" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="G9" s="12">
+      <c r="G9" s="11">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H9" s="12"/>
-    </row>
-    <row r="10" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="5" t="s">
+      <c r="H9" s="11"/>
+    </row>
+    <row r="10" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C10" s="12" t="s">
+      <c r="C10" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D10" s="12" t="s">
+      <c r="D10" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="E10" s="12" t="s">
+      <c r="E10" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="F10" s="12" t="s">
+      <c r="F10" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="G10" s="12">
+      <c r="G10" s="11">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="6" t="s">
+    <row r="11" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="D11" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E11" s="6" t="s">
+      <c r="E11" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="F11" s="6" t="s">
+      <c r="F11" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="G11" s="6">
+      <c r="G11" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="6" t="s">
+    <row r="12" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="D12" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="E12" s="6" t="s">
+      <c r="E12" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="F12" s="6" t="s">
+      <c r="F12" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="G12" s="6">
+      <c r="G12" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="6" t="s">
+    <row r="13" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="D13" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="E13" s="6" t="s">
+      <c r="E13" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="F13" s="6" t="s">
+      <c r="F13" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="G13" s="6">
+      <c r="G13" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="6" t="s">
+    <row r="14" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="C14" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D14" s="6" t="s">
+      <c r="D14" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="E14" s="6" t="s">
+      <c r="E14" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="F14" s="6" t="s">
+      <c r="F14" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="G14" s="6">
+      <c r="G14" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="6" t="s">
+    <row r="15" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="B15" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="C15" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D15" s="6" t="s">
+      <c r="D15" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E15" s="6" t="s">
+      <c r="E15" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="F15" s="6" t="s">
+      <c r="F15" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="G15" s="6">
+      <c r="G15" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="6" t="s">
+    <row r="16" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="B16" s="6" t="s">
+      <c r="B16" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="C16" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D16" s="6" t="s">
+      <c r="D16" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E16" s="6" t="s">
+      <c r="E16" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="F16" s="6" t="s">
+      <c r="F16" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="G16" s="6">
+      <c r="G16" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="7" t="s">
+    <row r="17" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B17" s="7" t="s">
+      <c r="B17" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C17" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="D17" s="7" t="s">
+      <c r="C17" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="D17" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="E17" s="7" t="s">
+      <c r="E17" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="F17" s="13" t="s">
+      <c r="F17" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="G17" s="13">
+      <c r="G17" s="12">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H17" s="13"/>
-    </row>
-    <row r="18" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="7" t="s">
+      <c r="H17" s="12"/>
+    </row>
+    <row r="18" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="7" t="s">
+      <c r="B18" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C18" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="D18" s="7" t="s">
+      <c r="C18" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="D18" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="E18" s="7" t="s">
+      <c r="E18" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="F18" s="13" t="s">
+      <c r="F18" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="G18" s="13">
+      <c r="G18" s="12">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H18" s="13"/>
-    </row>
-    <row r="19" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="7" t="s">
+      <c r="H18" s="12"/>
+    </row>
+    <row r="19" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B19" s="7" t="s">
+      <c r="B19" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C19" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="D19" s="7" t="s">
+      <c r="C19" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="D19" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="E19" s="7" t="s">
+      <c r="E19" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="F19" s="13" t="s">
+      <c r="F19" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="G19" s="13">
+      <c r="G19" s="12">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H19" s="13"/>
-    </row>
-    <row r="20" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="8" t="s">
+      <c r="H19" s="12"/>
+    </row>
+    <row r="20" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B20" s="8" t="s">
+      <c r="B20" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C20" s="8" t="s">
+      <c r="C20" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D20" s="8" t="s">
+      <c r="D20" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E20" s="8" t="s">
+      <c r="E20" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="F20" s="8" t="s">
+      <c r="F20" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="G20" s="8">
+      <c r="G20" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="9" t="s">
+    <row r="21" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B21" s="9" t="s">
+      <c r="B21" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="C21" s="9" t="s">
+      <c r="C21" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D21" s="9" t="s">
+      <c r="D21" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="E21" s="9" t="s">
+      <c r="E21" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="F21" s="14" t="s">
+      <c r="F21" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="G21" s="14">
+      <c r="G21" s="13">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="9" t="s">
+    <row r="22" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B22" s="9" t="s">
+      <c r="B22" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="C22" s="9" t="s">
+      <c r="C22" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D22" s="9" t="s">
+      <c r="D22" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="E22" s="9" t="s">
+      <c r="E22" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="F22" s="14" t="s">
+      <c r="F22" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="G22" s="14">
+      <c r="G22" s="13">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="9" t="s">
+    <row r="23" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B23" s="9" t="s">
+      <c r="B23" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="C23" s="9" t="s">
+      <c r="C23" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="D23" s="9" t="s">
+      <c r="D23" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="E23" s="9" t="s">
+      <c r="E23" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="F23" s="14" t="s">
+      <c r="F23" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="G23" s="14">
+      <c r="G23" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="9" t="s">
+    <row r="24" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B24" s="9" t="s">
+      <c r="B24" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="C24" s="9" t="s">
+      <c r="C24" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="D24" s="9" t="s">
+      <c r="D24" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="E24" s="9" t="s">
+      <c r="E24" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="F24" s="14" t="s">
+      <c r="F24" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="G24" s="14">
+      <c r="G24" s="13">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="9" t="s">
+    <row r="25" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B25" s="9" t="s">
+      <c r="B25" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="C25" s="9" t="s">
+      <c r="C25" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="D25" s="9" t="s">
+      <c r="D25" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="E25" s="9" t="s">
+      <c r="E25" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="F25" s="14" t="s">
+      <c r="F25" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="G25" s="14">
+      <c r="G25" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="9" t="s">
+    <row r="26" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B26" s="9" t="s">
+      <c r="B26" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="C26" s="9" t="s">
+      <c r="C26" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="D26" s="9" t="s">
+      <c r="D26" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="E26" s="9" t="s">
+      <c r="E26" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="F26" s="14" t="s">
+      <c r="F26" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="G26" s="14">
+      <c r="G26" s="13">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="9" t="s">
+    <row r="27" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B27" s="9" t="s">
+      <c r="B27" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="C27" s="9" t="s">
+      <c r="C27" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="D27" s="9" t="s">
+      <c r="D27" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="E27" s="9" t="s">
+      <c r="E27" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="F27" s="14" t="s">
+      <c r="F27" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="G27" s="14">
+      <c r="G27" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="9" t="s">
+    <row r="28" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B28" s="9" t="s">
+      <c r="B28" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="C28" s="9" t="s">
+      <c r="C28" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="D28" s="9" t="s">
+      <c r="D28" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="E28" s="9" t="s">
+      <c r="E28" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="F28" s="14" t="s">
+      <c r="F28" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="G28" s="14">
+      <c r="G28" s="13">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="9" t="s">
+    <row r="29" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B29" s="9" t="s">
+      <c r="B29" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="C29" s="9" t="s">
+      <c r="C29" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="D29" s="9" t="s">
+      <c r="D29" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="E29" s="9" t="s">
+      <c r="E29" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="F29" s="14" t="s">
+      <c r="F29" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="G29" s="14">
+      <c r="G29" s="13">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D30" s="1"/>
-      <c r="F30" s="15"/>
-      <c r="G30" s="15"/>
+      <c r="F30" s="14"/>
+      <c r="G30" s="14"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D31" s="1"/>
@@ -1916,8 +1915,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6956783-CD8A-4021-B812-DCE07115A14C}">
   <dimension ref="A1:I53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="B51" sqref="B2:B51"/>
+    <sheetView topLeftCell="A26" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1951,7 +1950,7 @@
       <c r="H1" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="I1" s="17" t="s">
+      <c r="I1" s="16" t="s">
         <v>107</v>
       </c>
     </row>
@@ -1959,25 +1958,25 @@
       <c r="A2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="C2" s="11">
-        <v>0.2</v>
-      </c>
-      <c r="D2" s="11">
-        <v>0</v>
-      </c>
-      <c r="E2" s="11">
-        <v>0</v>
-      </c>
-      <c r="F2" s="11">
-        <v>0</v>
-      </c>
-      <c r="G2" s="11">
-        <v>0</v>
-      </c>
-      <c r="H2" s="11">
+      <c r="C2" s="10">
+        <v>0.2</v>
+      </c>
+      <c r="D2" s="10">
+        <v>0</v>
+      </c>
+      <c r="E2" s="10">
+        <v>0</v>
+      </c>
+      <c r="F2" s="10">
+        <v>0</v>
+      </c>
+      <c r="G2" s="10">
+        <v>0</v>
+      </c>
+      <c r="H2" s="10">
         <v>1</v>
       </c>
       <c r="I2" s="1" t="s">
@@ -1988,25 +1987,25 @@
       <c r="A3" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="C3" s="11">
-        <v>0</v>
-      </c>
-      <c r="D3" s="11">
-        <v>0.2</v>
-      </c>
-      <c r="E3" s="11">
-        <v>0</v>
-      </c>
-      <c r="F3" s="11">
-        <v>0</v>
-      </c>
-      <c r="G3" s="11">
-        <v>0</v>
-      </c>
-      <c r="H3" s="11">
+      <c r="C3" s="10">
+        <v>0</v>
+      </c>
+      <c r="D3" s="10">
+        <v>0.2</v>
+      </c>
+      <c r="E3" s="10">
+        <v>0</v>
+      </c>
+      <c r="F3" s="10">
+        <v>0</v>
+      </c>
+      <c r="G3" s="10">
+        <v>0</v>
+      </c>
+      <c r="H3" s="10">
         <v>1</v>
       </c>
       <c r="I3" s="1" t="s">
@@ -2017,25 +2016,25 @@
       <c r="A4" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="C4" s="11">
-        <v>0</v>
-      </c>
-      <c r="D4" s="11">
-        <v>0</v>
-      </c>
-      <c r="E4" s="11">
-        <v>0.2</v>
-      </c>
-      <c r="F4" s="11">
-        <v>0</v>
-      </c>
-      <c r="G4" s="11">
-        <v>0</v>
-      </c>
-      <c r="H4" s="11">
+      <c r="C4" s="10">
+        <v>0</v>
+      </c>
+      <c r="D4" s="10">
+        <v>0</v>
+      </c>
+      <c r="E4" s="10">
+        <v>0.2</v>
+      </c>
+      <c r="F4" s="10">
+        <v>0</v>
+      </c>
+      <c r="G4" s="10">
+        <v>0</v>
+      </c>
+      <c r="H4" s="10">
         <v>1</v>
       </c>
       <c r="I4" s="1" t="s">
@@ -2046,25 +2045,25 @@
       <c r="A5" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="C5" s="11">
-        <v>0</v>
-      </c>
-      <c r="D5" s="11">
-        <v>0</v>
-      </c>
-      <c r="E5" s="11">
-        <v>0</v>
-      </c>
-      <c r="F5" s="11">
-        <v>0.2</v>
-      </c>
-      <c r="G5" s="11">
-        <v>0</v>
-      </c>
-      <c r="H5" s="11">
+      <c r="C5" s="10">
+        <v>0</v>
+      </c>
+      <c r="D5" s="10">
+        <v>0</v>
+      </c>
+      <c r="E5" s="10">
+        <v>0</v>
+      </c>
+      <c r="F5" s="10">
+        <v>0.2</v>
+      </c>
+      <c r="G5" s="10">
+        <v>0</v>
+      </c>
+      <c r="H5" s="10">
         <v>1</v>
       </c>
       <c r="I5" s="1" t="s">
@@ -2075,25 +2074,25 @@
       <c r="A6" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="C6" s="11">
-        <v>0</v>
-      </c>
-      <c r="D6" s="11">
-        <v>0</v>
-      </c>
-      <c r="E6" s="11">
-        <v>0</v>
-      </c>
-      <c r="F6" s="11">
-        <v>0</v>
-      </c>
-      <c r="G6" s="11">
-        <v>0.2</v>
-      </c>
-      <c r="H6" s="11">
+      <c r="C6" s="10">
+        <v>0</v>
+      </c>
+      <c r="D6" s="10">
+        <v>0</v>
+      </c>
+      <c r="E6" s="10">
+        <v>0</v>
+      </c>
+      <c r="F6" s="10">
+        <v>0</v>
+      </c>
+      <c r="G6" s="10">
+        <v>0.2</v>
+      </c>
+      <c r="H6" s="10">
         <v>1</v>
       </c>
       <c r="I6" s="1" t="s">
@@ -2104,25 +2103,25 @@
       <c r="A7" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="11">
-        <v>0.2</v>
-      </c>
-      <c r="D7" s="11">
-        <v>0.2</v>
-      </c>
-      <c r="E7" s="11">
-        <v>0.2</v>
-      </c>
-      <c r="F7" s="11">
-        <v>0.2</v>
-      </c>
-      <c r="G7" s="11">
-        <v>0.2</v>
-      </c>
-      <c r="H7" s="11">
+      <c r="C7" s="10">
+        <v>0.2</v>
+      </c>
+      <c r="D7" s="10">
+        <v>0.2</v>
+      </c>
+      <c r="E7" s="10">
+        <v>0.2</v>
+      </c>
+      <c r="F7" s="10">
+        <v>0.2</v>
+      </c>
+      <c r="G7" s="10">
+        <v>0.2</v>
+      </c>
+      <c r="H7" s="10">
         <v>5</v>
       </c>
       <c r="I7" s="1" t="s">
@@ -2133,25 +2132,25 @@
       <c r="A8" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="10" t="s">
         <v>103</v>
       </c>
-      <c r="C8" s="11">
-        <v>0.2</v>
-      </c>
-      <c r="D8" s="11">
-        <v>0.2</v>
-      </c>
-      <c r="E8" s="11">
-        <v>0</v>
-      </c>
-      <c r="F8" s="11">
-        <v>0</v>
-      </c>
-      <c r="G8" s="11">
-        <v>0</v>
-      </c>
-      <c r="H8" s="11">
+      <c r="C8" s="10">
+        <v>0.2</v>
+      </c>
+      <c r="D8" s="10">
+        <v>0.2</v>
+      </c>
+      <c r="E8" s="10">
+        <v>0</v>
+      </c>
+      <c r="F8" s="10">
+        <v>0</v>
+      </c>
+      <c r="G8" s="10">
+        <v>0</v>
+      </c>
+      <c r="H8" s="10">
         <v>2</v>
       </c>
       <c r="I8" s="1" t="s">
@@ -2162,25 +2161,25 @@
       <c r="A9" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="B9" s="11" t="s">
+      <c r="B9" s="10" t="s">
         <v>157</v>
       </c>
-      <c r="C9" s="11">
-        <v>0.2</v>
-      </c>
-      <c r="D9" s="11">
-        <v>0.2</v>
-      </c>
-      <c r="E9" s="11">
-        <v>0.2</v>
-      </c>
-      <c r="F9" s="11">
-        <v>0</v>
-      </c>
-      <c r="G9" s="11">
-        <v>0</v>
-      </c>
-      <c r="H9" s="11">
+      <c r="C9" s="10">
+        <v>0.2</v>
+      </c>
+      <c r="D9" s="10">
+        <v>0.2</v>
+      </c>
+      <c r="E9" s="10">
+        <v>0.2</v>
+      </c>
+      <c r="F9" s="10">
+        <v>0</v>
+      </c>
+      <c r="G9" s="10">
+        <v>0</v>
+      </c>
+      <c r="H9" s="10">
         <v>3</v>
       </c>
       <c r="I9" s="1" t="s">
@@ -2191,25 +2190,25 @@
       <c r="A10" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="B10" s="11" t="s">
+      <c r="B10" s="10" t="s">
         <v>163</v>
       </c>
-      <c r="C10" s="11">
-        <v>0.2</v>
-      </c>
-      <c r="D10" s="11">
-        <v>0.2</v>
-      </c>
-      <c r="E10" s="11">
-        <v>0.2</v>
-      </c>
-      <c r="F10" s="11">
-        <v>0.2</v>
-      </c>
-      <c r="G10" s="11">
-        <v>0</v>
-      </c>
-      <c r="H10" s="11">
+      <c r="C10" s="10">
+        <v>0.2</v>
+      </c>
+      <c r="D10" s="10">
+        <v>0.2</v>
+      </c>
+      <c r="E10" s="10">
+        <v>0.2</v>
+      </c>
+      <c r="F10" s="10">
+        <v>0.2</v>
+      </c>
+      <c r="G10" s="10">
+        <v>0</v>
+      </c>
+      <c r="H10" s="10">
         <v>4</v>
       </c>
       <c r="I10" s="1" t="s">
@@ -2220,25 +2219,25 @@
       <c r="A11" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="B11" s="11" t="s">
+      <c r="B11" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="C11" s="11">
-        <v>0.2</v>
-      </c>
-      <c r="D11" s="11">
-        <v>0</v>
-      </c>
-      <c r="E11" s="11">
-        <v>0.2</v>
-      </c>
-      <c r="F11" s="11">
-        <v>0</v>
-      </c>
-      <c r="G11" s="11">
-        <v>0</v>
-      </c>
-      <c r="H11" s="11">
+      <c r="C11" s="10">
+        <v>0.2</v>
+      </c>
+      <c r="D11" s="10">
+        <v>0</v>
+      </c>
+      <c r="E11" s="10">
+        <v>0.2</v>
+      </c>
+      <c r="F11" s="10">
+        <v>0</v>
+      </c>
+      <c r="G11" s="10">
+        <v>0</v>
+      </c>
+      <c r="H11" s="10">
         <v>2</v>
       </c>
       <c r="I11" s="1" t="s">
@@ -2249,25 +2248,25 @@
       <c r="A12" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="B12" s="11" t="s">
+      <c r="B12" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="C12" s="11">
-        <v>0.2</v>
-      </c>
-      <c r="D12" s="11">
-        <v>0</v>
-      </c>
-      <c r="E12" s="11">
-        <v>0</v>
-      </c>
-      <c r="F12" s="11">
-        <v>0.2</v>
-      </c>
-      <c r="G12" s="11">
-        <v>0</v>
-      </c>
-      <c r="H12" s="11">
+      <c r="C12" s="10">
+        <v>0.2</v>
+      </c>
+      <c r="D12" s="10">
+        <v>0</v>
+      </c>
+      <c r="E12" s="10">
+        <v>0</v>
+      </c>
+      <c r="F12" s="10">
+        <v>0.2</v>
+      </c>
+      <c r="G12" s="10">
+        <v>0</v>
+      </c>
+      <c r="H12" s="10">
         <v>2</v>
       </c>
       <c r="I12" s="1" t="s">
@@ -2278,25 +2277,25 @@
       <c r="A13" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="B13" s="11" t="s">
+      <c r="B13" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="C13" s="11">
-        <v>0.2</v>
-      </c>
-      <c r="D13" s="11">
-        <v>0</v>
-      </c>
-      <c r="E13" s="11">
-        <v>0</v>
-      </c>
-      <c r="F13" s="11">
-        <v>0</v>
-      </c>
-      <c r="G13" s="11">
-        <v>0.2</v>
-      </c>
-      <c r="H13" s="11">
+      <c r="C13" s="10">
+        <v>0.2</v>
+      </c>
+      <c r="D13" s="10">
+        <v>0</v>
+      </c>
+      <c r="E13" s="10">
+        <v>0</v>
+      </c>
+      <c r="F13" s="10">
+        <v>0</v>
+      </c>
+      <c r="G13" s="10">
+        <v>0.2</v>
+      </c>
+      <c r="H13" s="10">
         <v>2</v>
       </c>
       <c r="I13" s="1" t="s">
@@ -2307,25 +2306,25 @@
       <c r="A14" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="B14" s="11" t="s">
+      <c r="B14" s="10" t="s">
         <v>157</v>
       </c>
-      <c r="C14" s="11">
-        <v>0.2</v>
-      </c>
-      <c r="D14" s="11">
-        <v>0.2</v>
-      </c>
-      <c r="E14" s="11">
-        <v>0.2</v>
-      </c>
-      <c r="F14" s="11">
-        <v>0</v>
-      </c>
-      <c r="G14" s="11">
-        <v>0</v>
-      </c>
-      <c r="H14" s="11">
+      <c r="C14" s="10">
+        <v>0.2</v>
+      </c>
+      <c r="D14" s="10">
+        <v>0.2</v>
+      </c>
+      <c r="E14" s="10">
+        <v>0.2</v>
+      </c>
+      <c r="F14" s="10">
+        <v>0</v>
+      </c>
+      <c r="G14" s="10">
+        <v>0</v>
+      </c>
+      <c r="H14" s="10">
         <v>3</v>
       </c>
       <c r="I14" s="1" t="s">
@@ -2336,25 +2335,25 @@
       <c r="A15" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="B15" s="11" t="s">
+      <c r="B15" s="10" t="s">
         <v>163</v>
       </c>
-      <c r="C15" s="11">
-        <v>0.2</v>
-      </c>
-      <c r="D15" s="11">
-        <v>0.2</v>
-      </c>
-      <c r="E15" s="11">
-        <v>0.2</v>
-      </c>
-      <c r="F15" s="11">
-        <v>0.2</v>
-      </c>
-      <c r="G15" s="11">
-        <v>0</v>
-      </c>
-      <c r="H15" s="11">
+      <c r="C15" s="10">
+        <v>0.2</v>
+      </c>
+      <c r="D15" s="10">
+        <v>0.2</v>
+      </c>
+      <c r="E15" s="10">
+        <v>0.2</v>
+      </c>
+      <c r="F15" s="10">
+        <v>0.2</v>
+      </c>
+      <c r="G15" s="10">
+        <v>0</v>
+      </c>
+      <c r="H15" s="10">
         <v>4</v>
       </c>
       <c r="I15" s="1" t="s">
@@ -2365,25 +2364,25 @@
       <c r="A16" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="B16" s="11" t="s">
+      <c r="B16" s="10" t="s">
         <v>164</v>
       </c>
-      <c r="C16" s="11">
-        <v>0.2</v>
-      </c>
-      <c r="D16" s="11">
-        <v>0</v>
-      </c>
-      <c r="E16" s="11">
-        <v>0.2</v>
-      </c>
-      <c r="F16" s="11">
-        <v>0.2</v>
-      </c>
-      <c r="G16" s="11">
-        <v>0.2</v>
-      </c>
-      <c r="H16" s="11">
+      <c r="C16" s="10">
+        <v>0.2</v>
+      </c>
+      <c r="D16" s="10">
+        <v>0</v>
+      </c>
+      <c r="E16" s="10">
+        <v>0.2</v>
+      </c>
+      <c r="F16" s="10">
+        <v>0.2</v>
+      </c>
+      <c r="G16" s="10">
+        <v>0.2</v>
+      </c>
+      <c r="H16" s="10">
         <v>4</v>
       </c>
       <c r="I16" s="1" t="s">
@@ -2394,25 +2393,25 @@
       <c r="A17" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="B17" s="11" t="s">
+      <c r="B17" s="10" t="s">
         <v>158</v>
       </c>
-      <c r="C17" s="11">
-        <v>0.2</v>
-      </c>
-      <c r="D17" s="11">
-        <v>0</v>
-      </c>
-      <c r="E17" s="11">
-        <v>0.2</v>
-      </c>
-      <c r="F17" s="11">
-        <v>0</v>
-      </c>
-      <c r="G17" s="11">
-        <v>0.2</v>
-      </c>
-      <c r="H17" s="11">
+      <c r="C17" s="10">
+        <v>0.2</v>
+      </c>
+      <c r="D17" s="10">
+        <v>0</v>
+      </c>
+      <c r="E17" s="10">
+        <v>0.2</v>
+      </c>
+      <c r="F17" s="10">
+        <v>0</v>
+      </c>
+      <c r="G17" s="10">
+        <v>0.2</v>
+      </c>
+      <c r="H17" s="10">
         <v>3</v>
       </c>
       <c r="I17" s="1" t="s">
@@ -2423,25 +2422,25 @@
       <c r="A18" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="B18" s="11" t="s">
+      <c r="B18" s="10" t="s">
         <v>165</v>
       </c>
-      <c r="C18" s="11">
-        <v>0</v>
-      </c>
-      <c r="D18" s="11">
-        <v>0.2</v>
-      </c>
-      <c r="E18" s="11">
-        <v>0.2</v>
-      </c>
-      <c r="F18" s="11">
-        <v>0.2</v>
-      </c>
-      <c r="G18" s="11">
-        <v>0.2</v>
-      </c>
-      <c r="H18" s="11">
+      <c r="C18" s="10">
+        <v>0</v>
+      </c>
+      <c r="D18" s="10">
+        <v>0.2</v>
+      </c>
+      <c r="E18" s="10">
+        <v>0.2</v>
+      </c>
+      <c r="F18" s="10">
+        <v>0.2</v>
+      </c>
+      <c r="G18" s="10">
+        <v>0.2</v>
+      </c>
+      <c r="H18" s="10">
         <v>4</v>
       </c>
       <c r="I18" s="1" t="s">
@@ -2452,25 +2451,25 @@
       <c r="A19" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="B19" s="11" t="s">
+      <c r="B19" s="10" t="s">
         <v>162</v>
       </c>
-      <c r="C19" s="11">
-        <v>0</v>
-      </c>
-      <c r="D19" s="11">
-        <v>0</v>
-      </c>
-      <c r="E19" s="11">
-        <v>0.2</v>
-      </c>
-      <c r="F19" s="11">
-        <v>0.2</v>
-      </c>
-      <c r="G19" s="11">
-        <v>0.2</v>
-      </c>
-      <c r="H19" s="11">
+      <c r="C19" s="10">
+        <v>0</v>
+      </c>
+      <c r="D19" s="10">
+        <v>0</v>
+      </c>
+      <c r="E19" s="10">
+        <v>0.2</v>
+      </c>
+      <c r="F19" s="10">
+        <v>0.2</v>
+      </c>
+      <c r="G19" s="10">
+        <v>0.2</v>
+      </c>
+      <c r="H19" s="10">
         <v>3</v>
       </c>
       <c r="I19" s="1" t="s">
@@ -2481,25 +2480,25 @@
       <c r="A20" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="B20" s="11" t="s">
+      <c r="B20" s="10" t="s">
         <v>156</v>
       </c>
-      <c r="C20" s="11">
-        <v>0</v>
-      </c>
-      <c r="D20" s="11">
-        <v>0</v>
-      </c>
-      <c r="E20" s="11">
-        <v>0</v>
-      </c>
-      <c r="F20" s="11">
-        <v>0.2</v>
-      </c>
-      <c r="G20" s="11">
-        <v>0.2</v>
-      </c>
-      <c r="H20" s="11">
+      <c r="C20" s="10">
+        <v>0</v>
+      </c>
+      <c r="D20" s="10">
+        <v>0</v>
+      </c>
+      <c r="E20" s="10">
+        <v>0</v>
+      </c>
+      <c r="F20" s="10">
+        <v>0.2</v>
+      </c>
+      <c r="G20" s="10">
+        <v>0.2</v>
+      </c>
+      <c r="H20" s="10">
         <v>2</v>
       </c>
       <c r="I20" s="1" t="s">
@@ -2510,25 +2509,25 @@
       <c r="A21" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="B21" s="11" t="s">
+      <c r="B21" s="10" t="s">
         <v>160</v>
       </c>
-      <c r="C21" s="11">
-        <v>0</v>
-      </c>
-      <c r="D21" s="11">
-        <v>0.2</v>
-      </c>
-      <c r="E21" s="11">
-        <v>0.2</v>
-      </c>
-      <c r="F21" s="11">
-        <v>0</v>
-      </c>
-      <c r="G21" s="11">
-        <v>0.2</v>
-      </c>
-      <c r="H21" s="11">
+      <c r="C21" s="10">
+        <v>0</v>
+      </c>
+      <c r="D21" s="10">
+        <v>0.2</v>
+      </c>
+      <c r="E21" s="10">
+        <v>0.2</v>
+      </c>
+      <c r="F21" s="10">
+        <v>0</v>
+      </c>
+      <c r="G21" s="10">
+        <v>0.2</v>
+      </c>
+      <c r="H21" s="10">
         <v>3</v>
       </c>
       <c r="I21" s="1" t="s">
@@ -2539,25 +2538,25 @@
       <c r="A22" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="B22" s="11" t="s">
+      <c r="B22" s="10" t="s">
         <v>152</v>
       </c>
-      <c r="C22" s="11">
-        <v>0</v>
-      </c>
-      <c r="D22" s="11">
-        <v>0.2</v>
-      </c>
-      <c r="E22" s="11">
-        <v>0.2</v>
-      </c>
-      <c r="F22" s="11">
-        <v>0</v>
-      </c>
-      <c r="G22" s="11">
-        <v>0</v>
-      </c>
-      <c r="H22" s="11">
+      <c r="C22" s="10">
+        <v>0</v>
+      </c>
+      <c r="D22" s="10">
+        <v>0.2</v>
+      </c>
+      <c r="E22" s="10">
+        <v>0.2</v>
+      </c>
+      <c r="F22" s="10">
+        <v>0</v>
+      </c>
+      <c r="G22" s="10">
+        <v>0</v>
+      </c>
+      <c r="H22" s="10">
         <v>2</v>
       </c>
       <c r="I22" s="1" t="s">
@@ -2568,25 +2567,25 @@
       <c r="A23" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="B23" s="11" t="s">
+      <c r="B23" s="10" t="s">
         <v>155</v>
       </c>
-      <c r="C23" s="11">
-        <v>0</v>
-      </c>
-      <c r="D23" s="11">
-        <v>0</v>
-      </c>
-      <c r="E23" s="11">
-        <v>0.2</v>
-      </c>
-      <c r="F23" s="11">
-        <v>0</v>
-      </c>
-      <c r="G23" s="11">
-        <v>0.2</v>
-      </c>
-      <c r="H23" s="11">
+      <c r="C23" s="10">
+        <v>0</v>
+      </c>
+      <c r="D23" s="10">
+        <v>0</v>
+      </c>
+      <c r="E23" s="10">
+        <v>0.2</v>
+      </c>
+      <c r="F23" s="10">
+        <v>0</v>
+      </c>
+      <c r="G23" s="10">
+        <v>0.2</v>
+      </c>
+      <c r="H23" s="10">
         <v>2</v>
       </c>
       <c r="I23" s="1" t="s">
@@ -2597,25 +2596,25 @@
       <c r="A24" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="B24" s="11" t="s">
+      <c r="B24" s="10" t="s">
         <v>154</v>
       </c>
-      <c r="C24" s="11">
-        <v>0</v>
-      </c>
-      <c r="D24" s="11">
-        <v>0</v>
-      </c>
-      <c r="E24" s="11">
-        <v>0.2</v>
-      </c>
-      <c r="F24" s="11">
-        <v>0.2</v>
-      </c>
-      <c r="G24" s="11">
-        <v>0</v>
-      </c>
-      <c r="H24" s="11">
+      <c r="C24" s="10">
+        <v>0</v>
+      </c>
+      <c r="D24" s="10">
+        <v>0</v>
+      </c>
+      <c r="E24" s="10">
+        <v>0.2</v>
+      </c>
+      <c r="F24" s="10">
+        <v>0.2</v>
+      </c>
+      <c r="G24" s="10">
+        <v>0</v>
+      </c>
+      <c r="H24" s="10">
         <v>2</v>
       </c>
       <c r="I24" s="1" t="s">
@@ -2626,25 +2625,25 @@
       <c r="A25" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="B25" s="11" t="s">
+      <c r="B25" s="10" t="s">
         <v>161</v>
       </c>
-      <c r="C25" s="11">
-        <v>0</v>
-      </c>
-      <c r="D25" s="11">
-        <v>0.2</v>
-      </c>
-      <c r="E25" s="11">
-        <v>0</v>
-      </c>
-      <c r="F25" s="11">
-        <v>0.2</v>
-      </c>
-      <c r="G25" s="11">
-        <v>0.2</v>
-      </c>
-      <c r="H25" s="11">
+      <c r="C25" s="10">
+        <v>0</v>
+      </c>
+      <c r="D25" s="10">
+        <v>0.2</v>
+      </c>
+      <c r="E25" s="10">
+        <v>0</v>
+      </c>
+      <c r="F25" s="10">
+        <v>0.2</v>
+      </c>
+      <c r="G25" s="10">
+        <v>0.2</v>
+      </c>
+      <c r="H25" s="10">
         <v>3</v>
       </c>
       <c r="I25" s="1" t="s">
@@ -2655,25 +2654,25 @@
       <c r="A26" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="B26" s="11" t="s">
+      <c r="B26" s="10" t="s">
         <v>153</v>
       </c>
-      <c r="C26" s="11">
-        <v>0</v>
-      </c>
-      <c r="D26" s="11">
-        <v>0.2</v>
-      </c>
-      <c r="E26" s="11">
-        <v>0</v>
-      </c>
-      <c r="F26" s="11">
-        <v>0.2</v>
-      </c>
-      <c r="G26" s="11">
-        <v>0</v>
-      </c>
-      <c r="H26" s="11">
+      <c r="C26" s="10">
+        <v>0</v>
+      </c>
+      <c r="D26" s="10">
+        <v>0.2</v>
+      </c>
+      <c r="E26" s="10">
+        <v>0</v>
+      </c>
+      <c r="F26" s="10">
+        <v>0.2</v>
+      </c>
+      <c r="G26" s="10">
+        <v>0</v>
+      </c>
+      <c r="H26" s="10">
         <v>2</v>
       </c>
       <c r="I26" s="1" t="s">
@@ -2684,25 +2683,25 @@
       <c r="A27" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="B27" s="11" t="s">
+      <c r="B27" s="10" t="s">
         <v>159</v>
       </c>
-      <c r="C27" s="11">
-        <v>0</v>
-      </c>
-      <c r="D27" s="11">
-        <v>0.2</v>
-      </c>
-      <c r="E27" s="11">
-        <v>0.2</v>
-      </c>
-      <c r="F27" s="11">
-        <v>0.2</v>
-      </c>
-      <c r="G27" s="11">
-        <v>0</v>
-      </c>
-      <c r="H27" s="11">
+      <c r="C27" s="10">
+        <v>0</v>
+      </c>
+      <c r="D27" s="10">
+        <v>0.2</v>
+      </c>
+      <c r="E27" s="10">
+        <v>0.2</v>
+      </c>
+      <c r="F27" s="10">
+        <v>0.2</v>
+      </c>
+      <c r="G27" s="10">
+        <v>0</v>
+      </c>
+      <c r="H27" s="10">
         <v>3</v>
       </c>
       <c r="I27" s="1" t="s">
@@ -2713,25 +2712,25 @@
       <c r="A28" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="B28" s="11" t="s">
+      <c r="B28" s="10" t="s">
         <v>168</v>
       </c>
-      <c r="C28" s="11">
+      <c r="C28" s="10">
         <v>0.4</v>
       </c>
-      <c r="D28" s="11">
-        <v>0.2</v>
-      </c>
-      <c r="E28" s="11">
-        <v>0</v>
-      </c>
-      <c r="F28" s="11">
-        <v>0</v>
-      </c>
-      <c r="G28" s="11">
-        <v>0</v>
-      </c>
-      <c r="H28" s="11">
+      <c r="D28" s="10">
+        <v>0.2</v>
+      </c>
+      <c r="E28" s="10">
+        <v>0</v>
+      </c>
+      <c r="F28" s="10">
+        <v>0</v>
+      </c>
+      <c r="G28" s="10">
+        <v>0</v>
+      </c>
+      <c r="H28" s="10">
         <v>2</v>
       </c>
       <c r="I28" s="1" t="s">
@@ -2742,25 +2741,25 @@
       <c r="A29" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="B29" s="11" t="s">
+      <c r="B29" s="10" t="s">
         <v>170</v>
       </c>
-      <c r="C29" s="11">
+      <c r="C29" s="10">
         <v>0.4</v>
       </c>
-      <c r="D29" s="11">
-        <v>0</v>
-      </c>
-      <c r="E29" s="11">
-        <v>0.2</v>
-      </c>
-      <c r="F29" s="11">
-        <v>0</v>
-      </c>
-      <c r="G29" s="11">
-        <v>0</v>
-      </c>
-      <c r="H29" s="11">
+      <c r="D29" s="10">
+        <v>0</v>
+      </c>
+      <c r="E29" s="10">
+        <v>0.2</v>
+      </c>
+      <c r="F29" s="10">
+        <v>0</v>
+      </c>
+      <c r="G29" s="10">
+        <v>0</v>
+      </c>
+      <c r="H29" s="10">
         <v>2</v>
       </c>
       <c r="I29" s="1" t="s">
@@ -2771,25 +2770,25 @@
       <c r="A30" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="B30" s="11" t="s">
+      <c r="B30" s="10" t="s">
         <v>172</v>
       </c>
-      <c r="C30" s="11">
+      <c r="C30" s="10">
         <v>0.4</v>
       </c>
-      <c r="D30" s="11">
-        <v>0</v>
-      </c>
-      <c r="E30" s="11">
-        <v>0</v>
-      </c>
-      <c r="F30" s="11">
-        <v>0.2</v>
-      </c>
-      <c r="G30" s="11">
-        <v>0</v>
-      </c>
-      <c r="H30" s="11">
+      <c r="D30" s="10">
+        <v>0</v>
+      </c>
+      <c r="E30" s="10">
+        <v>0</v>
+      </c>
+      <c r="F30" s="10">
+        <v>0.2</v>
+      </c>
+      <c r="G30" s="10">
+        <v>0</v>
+      </c>
+      <c r="H30" s="10">
         <v>2</v>
       </c>
       <c r="I30" s="1" t="s">
@@ -2800,25 +2799,25 @@
       <c r="A31" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="B31" s="11" t="s">
+      <c r="B31" s="10" t="s">
         <v>174</v>
       </c>
-      <c r="C31" s="11">
+      <c r="C31" s="10">
         <v>0.4</v>
       </c>
-      <c r="D31" s="11">
-        <v>0</v>
-      </c>
-      <c r="E31" s="11">
-        <v>0</v>
-      </c>
-      <c r="F31" s="11">
-        <v>0</v>
-      </c>
-      <c r="G31" s="11">
-        <v>0.2</v>
-      </c>
-      <c r="H31" s="11">
+      <c r="D31" s="10">
+        <v>0</v>
+      </c>
+      <c r="E31" s="10">
+        <v>0</v>
+      </c>
+      <c r="F31" s="10">
+        <v>0</v>
+      </c>
+      <c r="G31" s="10">
+        <v>0.2</v>
+      </c>
+      <c r="H31" s="10">
         <v>2</v>
       </c>
       <c r="I31" s="1" t="s">
@@ -2829,25 +2828,25 @@
       <c r="A32" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="B32" s="11" t="s">
+      <c r="B32" s="10" t="s">
         <v>176</v>
       </c>
-      <c r="C32" s="11">
-        <v>0.2</v>
-      </c>
-      <c r="D32" s="11">
+      <c r="C32" s="10">
+        <v>0.2</v>
+      </c>
+      <c r="D32" s="10">
         <v>0.4</v>
       </c>
-      <c r="E32" s="11">
-        <v>0</v>
-      </c>
-      <c r="F32" s="11">
-        <v>0</v>
-      </c>
-      <c r="G32" s="11">
-        <v>0</v>
-      </c>
-      <c r="H32" s="11">
+      <c r="E32" s="10">
+        <v>0</v>
+      </c>
+      <c r="F32" s="10">
+        <v>0</v>
+      </c>
+      <c r="G32" s="10">
+        <v>0</v>
+      </c>
+      <c r="H32" s="10">
         <v>2</v>
       </c>
       <c r="I32" s="1" t="s">
@@ -2858,25 +2857,25 @@
       <c r="A33" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="B33" s="11" t="s">
+      <c r="B33" s="10" t="s">
         <v>178</v>
       </c>
-      <c r="C33" s="11">
-        <v>0</v>
-      </c>
-      <c r="D33" s="11">
+      <c r="C33" s="10">
+        <v>0</v>
+      </c>
+      <c r="D33" s="10">
         <v>0.4</v>
       </c>
-      <c r="E33" s="11">
-        <v>0.2</v>
-      </c>
-      <c r="F33" s="11">
-        <v>0</v>
-      </c>
-      <c r="G33" s="11">
-        <v>0</v>
-      </c>
-      <c r="H33" s="11">
+      <c r="E33" s="10">
+        <v>0.2</v>
+      </c>
+      <c r="F33" s="10">
+        <v>0</v>
+      </c>
+      <c r="G33" s="10">
+        <v>0</v>
+      </c>
+      <c r="H33" s="10">
         <v>2</v>
       </c>
       <c r="I33" s="1" t="s">
@@ -2887,25 +2886,25 @@
       <c r="A34" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="B34" s="11" t="s">
+      <c r="B34" s="10" t="s">
         <v>180</v>
       </c>
-      <c r="C34" s="11">
-        <v>0</v>
-      </c>
-      <c r="D34" s="11">
+      <c r="C34" s="10">
+        <v>0</v>
+      </c>
+      <c r="D34" s="10">
         <v>0.4</v>
       </c>
-      <c r="E34" s="11">
-        <v>0</v>
-      </c>
-      <c r="F34" s="11">
-        <v>0.2</v>
-      </c>
-      <c r="G34" s="11">
-        <v>0</v>
-      </c>
-      <c r="H34" s="11">
+      <c r="E34" s="10">
+        <v>0</v>
+      </c>
+      <c r="F34" s="10">
+        <v>0.2</v>
+      </c>
+      <c r="G34" s="10">
+        <v>0</v>
+      </c>
+      <c r="H34" s="10">
         <v>2</v>
       </c>
       <c r="I34" s="1" t="s">
@@ -2916,25 +2915,25 @@
       <c r="A35" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="B35" s="11" t="s">
+      <c r="B35" s="10" t="s">
         <v>182</v>
       </c>
-      <c r="C35" s="11">
-        <v>0</v>
-      </c>
-      <c r="D35" s="11">
+      <c r="C35" s="10">
+        <v>0</v>
+      </c>
+      <c r="D35" s="10">
         <v>0.4</v>
       </c>
-      <c r="E35" s="11">
-        <v>0</v>
-      </c>
-      <c r="F35" s="11">
-        <v>0</v>
-      </c>
-      <c r="G35" s="11">
-        <v>0.2</v>
-      </c>
-      <c r="H35" s="11">
+      <c r="E35" s="10">
+        <v>0</v>
+      </c>
+      <c r="F35" s="10">
+        <v>0</v>
+      </c>
+      <c r="G35" s="10">
+        <v>0.2</v>
+      </c>
+      <c r="H35" s="10">
         <v>2</v>
       </c>
       <c r="I35" s="1" t="s">
@@ -2945,25 +2944,25 @@
       <c r="A36" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="B36" s="11" t="s">
+      <c r="B36" s="10" t="s">
         <v>184</v>
       </c>
-      <c r="C36" s="11">
-        <v>0.2</v>
-      </c>
-      <c r="D36" s="11">
-        <v>0</v>
-      </c>
-      <c r="E36" s="11">
+      <c r="C36" s="10">
+        <v>0.2</v>
+      </c>
+      <c r="D36" s="10">
+        <v>0</v>
+      </c>
+      <c r="E36" s="10">
         <v>0.4</v>
       </c>
-      <c r="F36" s="11">
-        <v>0</v>
-      </c>
-      <c r="G36" s="11">
-        <v>0</v>
-      </c>
-      <c r="H36" s="11">
+      <c r="F36" s="10">
+        <v>0</v>
+      </c>
+      <c r="G36" s="10">
+        <v>0</v>
+      </c>
+      <c r="H36" s="10">
         <v>2</v>
       </c>
       <c r="I36" s="1" t="s">
@@ -2974,25 +2973,25 @@
       <c r="A37" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="B37" s="11" t="s">
+      <c r="B37" s="10" t="s">
         <v>186</v>
       </c>
-      <c r="C37" s="11">
-        <v>0</v>
-      </c>
-      <c r="D37" s="11">
-        <v>0.2</v>
-      </c>
-      <c r="E37" s="11">
+      <c r="C37" s="10">
+        <v>0</v>
+      </c>
+      <c r="D37" s="10">
+        <v>0.2</v>
+      </c>
+      <c r="E37" s="10">
         <v>0.4</v>
       </c>
-      <c r="F37" s="11">
-        <v>0</v>
-      </c>
-      <c r="G37" s="11">
-        <v>0</v>
-      </c>
-      <c r="H37" s="11">
+      <c r="F37" s="10">
+        <v>0</v>
+      </c>
+      <c r="G37" s="10">
+        <v>0</v>
+      </c>
+      <c r="H37" s="10">
         <v>2</v>
       </c>
       <c r="I37" s="1" t="s">
@@ -3003,25 +3002,25 @@
       <c r="A38" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="B38" s="11" t="s">
+      <c r="B38" s="10" t="s">
         <v>194</v>
       </c>
-      <c r="C38" s="11">
-        <v>0</v>
-      </c>
-      <c r="D38" s="11">
-        <v>0</v>
-      </c>
-      <c r="E38" s="11">
+      <c r="C38" s="10">
+        <v>0</v>
+      </c>
+      <c r="D38" s="10">
+        <v>0</v>
+      </c>
+      <c r="E38" s="10">
         <v>0.4</v>
       </c>
-      <c r="F38" s="11">
-        <v>0.2</v>
-      </c>
-      <c r="G38" s="11">
-        <v>0</v>
-      </c>
-      <c r="H38" s="11">
+      <c r="F38" s="10">
+        <v>0.2</v>
+      </c>
+      <c r="G38" s="10">
+        <v>0</v>
+      </c>
+      <c r="H38" s="10">
         <v>2</v>
       </c>
       <c r="I38" s="1" t="s">
@@ -3032,25 +3031,25 @@
       <c r="A39" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="B39" s="11" t="s">
+      <c r="B39" s="10" t="s">
         <v>197</v>
       </c>
-      <c r="C39" s="11">
-        <v>0</v>
-      </c>
-      <c r="D39" s="11">
-        <v>0</v>
-      </c>
-      <c r="E39" s="11">
+      <c r="C39" s="10">
+        <v>0</v>
+      </c>
+      <c r="D39" s="10">
+        <v>0</v>
+      </c>
+      <c r="E39" s="10">
         <v>0.4</v>
       </c>
-      <c r="F39" s="11">
-        <v>0</v>
-      </c>
-      <c r="G39" s="11">
-        <v>0.2</v>
-      </c>
-      <c r="H39" s="11">
+      <c r="F39" s="10">
+        <v>0</v>
+      </c>
+      <c r="G39" s="10">
+        <v>0.2</v>
+      </c>
+      <c r="H39" s="10">
         <v>2</v>
       </c>
       <c r="I39" s="1" t="s">
@@ -3061,25 +3060,25 @@
       <c r="A40" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="B40" s="11" t="s">
+      <c r="B40" s="10" t="s">
         <v>199</v>
       </c>
-      <c r="C40" s="11">
-        <v>0.2</v>
-      </c>
-      <c r="D40" s="11">
-        <v>0</v>
-      </c>
-      <c r="E40" s="11">
-        <v>0</v>
-      </c>
-      <c r="F40" s="11">
+      <c r="C40" s="10">
+        <v>0.2</v>
+      </c>
+      <c r="D40" s="10">
+        <v>0</v>
+      </c>
+      <c r="E40" s="10">
+        <v>0</v>
+      </c>
+      <c r="F40" s="10">
         <v>0.4</v>
       </c>
-      <c r="G40" s="11">
-        <v>0</v>
-      </c>
-      <c r="H40" s="11">
+      <c r="G40" s="10">
+        <v>0</v>
+      </c>
+      <c r="H40" s="10">
         <v>2</v>
       </c>
       <c r="I40" s="1" t="s">
@@ -3090,25 +3089,25 @@
       <c r="A41" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="B41" s="11" t="s">
+      <c r="B41" s="10" t="s">
         <v>201</v>
       </c>
-      <c r="C41" s="11">
-        <v>0</v>
-      </c>
-      <c r="D41" s="11">
-        <v>0.2</v>
-      </c>
-      <c r="E41" s="11">
-        <v>0</v>
-      </c>
-      <c r="F41" s="11">
+      <c r="C41" s="10">
+        <v>0</v>
+      </c>
+      <c r="D41" s="10">
+        <v>0.2</v>
+      </c>
+      <c r="E41" s="10">
+        <v>0</v>
+      </c>
+      <c r="F41" s="10">
         <v>0.4</v>
       </c>
-      <c r="G41" s="11">
-        <v>0</v>
-      </c>
-      <c r="H41" s="11">
+      <c r="G41" s="10">
+        <v>0</v>
+      </c>
+      <c r="H41" s="10">
         <v>2</v>
       </c>
       <c r="I41" s="1" t="s">
@@ -3119,25 +3118,25 @@
       <c r="A42" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="B42" s="11" t="s">
+      <c r="B42" s="10" t="s">
         <v>203</v>
       </c>
-      <c r="C42" s="11">
-        <v>0</v>
-      </c>
-      <c r="D42" s="11">
-        <v>0</v>
-      </c>
-      <c r="E42" s="11">
-        <v>0.2</v>
-      </c>
-      <c r="F42" s="11">
+      <c r="C42" s="10">
+        <v>0</v>
+      </c>
+      <c r="D42" s="10">
+        <v>0</v>
+      </c>
+      <c r="E42" s="10">
+        <v>0.2</v>
+      </c>
+      <c r="F42" s="10">
         <v>0.4</v>
       </c>
-      <c r="G42" s="11">
-        <v>0</v>
-      </c>
-      <c r="H42" s="11">
+      <c r="G42" s="10">
+        <v>0</v>
+      </c>
+      <c r="H42" s="10">
         <v>2</v>
       </c>
       <c r="I42" s="1" t="s">
@@ -3148,25 +3147,25 @@
       <c r="A43" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="B43" s="11" t="s">
+      <c r="B43" s="10" t="s">
         <v>205</v>
       </c>
-      <c r="C43" s="11">
-        <v>0</v>
-      </c>
-      <c r="D43" s="11">
-        <v>0</v>
-      </c>
-      <c r="E43" s="11">
-        <v>0</v>
-      </c>
-      <c r="F43" s="11">
+      <c r="C43" s="10">
+        <v>0</v>
+      </c>
+      <c r="D43" s="10">
+        <v>0</v>
+      </c>
+      <c r="E43" s="10">
+        <v>0</v>
+      </c>
+      <c r="F43" s="10">
         <v>0.4</v>
       </c>
-      <c r="G43" s="11">
-        <v>0.2</v>
-      </c>
-      <c r="H43" s="11">
+      <c r="G43" s="10">
+        <v>0.2</v>
+      </c>
+      <c r="H43" s="10">
         <v>2</v>
       </c>
       <c r="I43" s="1" t="s">
@@ -3177,25 +3176,25 @@
       <c r="A44" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="B44" s="11" t="s">
+      <c r="B44" s="10" t="s">
         <v>207</v>
       </c>
-      <c r="C44" s="11">
-        <v>0.2</v>
-      </c>
-      <c r="D44" s="11">
-        <v>0</v>
-      </c>
-      <c r="E44" s="11">
-        <v>0</v>
-      </c>
-      <c r="F44" s="11">
-        <v>0</v>
-      </c>
-      <c r="G44" s="11">
+      <c r="C44" s="10">
+        <v>0.2</v>
+      </c>
+      <c r="D44" s="10">
+        <v>0</v>
+      </c>
+      <c r="E44" s="10">
+        <v>0</v>
+      </c>
+      <c r="F44" s="10">
+        <v>0</v>
+      </c>
+      <c r="G44" s="10">
         <v>0.4</v>
       </c>
-      <c r="H44" s="11">
+      <c r="H44" s="10">
         <v>2</v>
       </c>
       <c r="I44" s="1" t="s">
@@ -3206,25 +3205,25 @@
       <c r="A45" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="B45" s="11" t="s">
+      <c r="B45" s="10" t="s">
         <v>216</v>
       </c>
-      <c r="C45" s="11">
-        <v>0</v>
-      </c>
-      <c r="D45" s="11">
-        <v>0.2</v>
-      </c>
-      <c r="E45" s="11">
-        <v>0</v>
-      </c>
-      <c r="F45" s="11">
-        <v>0</v>
-      </c>
-      <c r="G45" s="11">
+      <c r="C45" s="10">
+        <v>0</v>
+      </c>
+      <c r="D45" s="10">
+        <v>0.2</v>
+      </c>
+      <c r="E45" s="10">
+        <v>0</v>
+      </c>
+      <c r="F45" s="10">
+        <v>0</v>
+      </c>
+      <c r="G45" s="10">
         <v>0.4</v>
       </c>
-      <c r="H45" s="11">
+      <c r="H45" s="10">
         <v>2</v>
       </c>
       <c r="I45" s="1" t="s">
@@ -3235,25 +3234,25 @@
       <c r="A46" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="B46" s="11" t="s">
+      <c r="B46" s="10" t="s">
         <v>218</v>
       </c>
-      <c r="C46" s="11">
-        <v>0</v>
-      </c>
-      <c r="D46" s="11">
-        <v>0</v>
-      </c>
-      <c r="E46" s="11">
-        <v>0.2</v>
-      </c>
-      <c r="F46" s="11">
-        <v>0</v>
-      </c>
-      <c r="G46" s="11">
+      <c r="C46" s="10">
+        <v>0</v>
+      </c>
+      <c r="D46" s="10">
+        <v>0</v>
+      </c>
+      <c r="E46" s="10">
+        <v>0.2</v>
+      </c>
+      <c r="F46" s="10">
+        <v>0</v>
+      </c>
+      <c r="G46" s="10">
         <v>0.4</v>
       </c>
-      <c r="H46" s="11">
+      <c r="H46" s="10">
         <v>2</v>
       </c>
       <c r="I46" s="1" t="s">
@@ -3264,25 +3263,25 @@
       <c r="A47" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="B47" s="11" t="s">
+      <c r="B47" s="10" t="s">
         <v>220</v>
       </c>
-      <c r="C47" s="11">
-        <v>0</v>
-      </c>
-      <c r="D47" s="11">
-        <v>0</v>
-      </c>
-      <c r="E47" s="11">
-        <v>0</v>
-      </c>
-      <c r="F47" s="11">
-        <v>0.2</v>
-      </c>
-      <c r="G47" s="11">
+      <c r="C47" s="10">
+        <v>0</v>
+      </c>
+      <c r="D47" s="10">
+        <v>0</v>
+      </c>
+      <c r="E47" s="10">
+        <v>0</v>
+      </c>
+      <c r="F47" s="10">
+        <v>0.2</v>
+      </c>
+      <c r="G47" s="10">
         <v>0.4</v>
       </c>
-      <c r="H47" s="11">
+      <c r="H47" s="10">
         <v>2</v>
       </c>
       <c r="I47" s="1" t="s">
@@ -3293,25 +3292,25 @@
       <c r="A48" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="B48" s="11" t="s">
+      <c r="B48" s="10" t="s">
         <v>222</v>
       </c>
-      <c r="C48" s="11">
-        <v>0</v>
-      </c>
-      <c r="D48" s="11">
-        <v>0.2</v>
-      </c>
-      <c r="E48" s="11">
+      <c r="C48" s="10">
+        <v>0</v>
+      </c>
+      <c r="D48" s="10">
+        <v>0.2</v>
+      </c>
+      <c r="E48" s="10">
         <v>0.4</v>
       </c>
-      <c r="F48" s="11">
-        <v>0.2</v>
-      </c>
-      <c r="G48" s="11">
+      <c r="F48" s="10">
+        <v>0.2</v>
+      </c>
+      <c r="G48" s="10">
         <v>0.4</v>
       </c>
-      <c r="H48" s="11">
+      <c r="H48" s="10">
         <v>4</v>
       </c>
       <c r="I48" s="1" t="s">
@@ -3322,25 +3321,25 @@
       <c r="A49" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="B49" s="11" t="s">
+      <c r="B49" s="10" t="s">
         <v>224</v>
       </c>
-      <c r="C49" s="11">
-        <v>0</v>
-      </c>
-      <c r="D49" s="11">
+      <c r="C49" s="10">
+        <v>0</v>
+      </c>
+      <c r="D49" s="10">
         <v>0.4</v>
       </c>
-      <c r="E49" s="11">
-        <v>0.2</v>
-      </c>
-      <c r="F49" s="11">
+      <c r="E49" s="10">
+        <v>0.2</v>
+      </c>
+      <c r="F49" s="10">
         <v>0.4</v>
       </c>
-      <c r="G49" s="11">
-        <v>0.2</v>
-      </c>
-      <c r="H49" s="11">
+      <c r="G49" s="10">
+        <v>0.2</v>
+      </c>
+      <c r="H49" s="10">
         <v>4</v>
       </c>
       <c r="I49" s="1" t="s">
@@ -3351,25 +3350,25 @@
       <c r="A50" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="B50" s="11" t="s">
+      <c r="B50" s="10" t="s">
         <v>226</v>
       </c>
-      <c r="C50" s="11">
-        <v>0</v>
-      </c>
-      <c r="D50" s="11">
+      <c r="C50" s="10">
+        <v>0</v>
+      </c>
+      <c r="D50" s="10">
         <v>0.4</v>
       </c>
-      <c r="E50" s="11">
+      <c r="E50" s="10">
         <v>0.4</v>
       </c>
-      <c r="F50" s="11">
-        <v>0.2</v>
-      </c>
-      <c r="G50" s="11">
-        <v>0.2</v>
-      </c>
-      <c r="H50" s="11">
+      <c r="F50" s="10">
+        <v>0.2</v>
+      </c>
+      <c r="G50" s="10">
+        <v>0.2</v>
+      </c>
+      <c r="H50" s="10">
         <v>4</v>
       </c>
       <c r="I50" s="1" t="s">
@@ -3380,25 +3379,25 @@
       <c r="A51" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="B51" s="11" t="s">
+      <c r="B51" s="10" t="s">
         <v>228</v>
       </c>
-      <c r="C51" s="11">
-        <v>0</v>
-      </c>
-      <c r="D51" s="11">
-        <v>0.2</v>
-      </c>
-      <c r="E51" s="11">
+      <c r="C51" s="10">
+        <v>0</v>
+      </c>
+      <c r="D51" s="10">
+        <v>0.2</v>
+      </c>
+      <c r="E51" s="10">
         <v>0.4</v>
       </c>
-      <c r="F51" s="11">
+      <c r="F51" s="10">
         <v>0.4</v>
       </c>
-      <c r="G51" s="11">
-        <v>0.2</v>
-      </c>
-      <c r="H51" s="11">
+      <c r="G51" s="10">
+        <v>0.2</v>
+      </c>
+      <c r="H51" s="10">
         <v>4</v>
       </c>
       <c r="I51" s="1" t="s">
@@ -3419,269 +3418,183 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCC343D5-ACEC-440C-BE2B-40BCC1E75BAA}">
-  <dimension ref="A1:AB3"/>
+  <dimension ref="A1:AB2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="G1" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="H1" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="I1" s="10" t="s">
+      <c r="I1" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="J1" s="10" t="s">
+      <c r="J1" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="K1" s="10" t="s">
+      <c r="K1" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="L1" s="10" t="s">
+      <c r="L1" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="M1" s="10" t="s">
+      <c r="M1" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="N1" s="10" t="s">
+      <c r="N1" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="O1" s="10" t="s">
+      <c r="O1" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="P1" s="10" t="s">
+      <c r="P1" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="Q1" s="10" t="s">
+      <c r="Q1" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="R1" s="10" t="s">
+      <c r="R1" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="S1" s="10" t="s">
+      <c r="S1" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="T1" s="10" t="s">
+      <c r="T1" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="U1" s="10" t="s">
+      <c r="U1" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="V1" s="10" t="s">
+      <c r="V1" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="W1" s="10" t="s">
+      <c r="W1" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="X1" s="10" t="s">
+      <c r="X1" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="Y1" s="10" t="s">
+      <c r="Y1" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="Z1" s="10" t="s">
+      <c r="Z1" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="AA1" s="10" t="s">
+      <c r="AA1" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="AB1" s="10" t="s">
+      <c r="AB1" s="9" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="O2" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="P2" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q2" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="R2" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="S2" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="T2" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="U2" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="V2" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="W2" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="X2" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="Y2" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="Z2" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="AA2" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="AB2" s="3" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="3" spans="1:28" s="16" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="16">
-        <v>1</v>
-      </c>
-      <c r="B3" s="16">
-        <v>1</v>
-      </c>
-      <c r="C3" s="16">
-        <v>1</v>
-      </c>
-      <c r="D3" s="16">
-        <v>1</v>
-      </c>
-      <c r="E3" s="16">
-        <v>1</v>
-      </c>
-      <c r="F3" s="16">
-        <v>1</v>
-      </c>
-      <c r="G3" s="16">
-        <v>1</v>
-      </c>
-      <c r="H3" s="16">
-        <v>1</v>
-      </c>
-      <c r="I3" s="16">
-        <v>1</v>
-      </c>
-      <c r="J3" s="16">
-        <v>1</v>
-      </c>
-      <c r="K3" s="16">
-        <v>1</v>
-      </c>
-      <c r="L3" s="16">
-        <v>1</v>
-      </c>
-      <c r="M3" s="16">
-        <v>1</v>
-      </c>
-      <c r="N3" s="16">
-        <v>1</v>
-      </c>
-      <c r="O3" s="16">
-        <v>0</v>
-      </c>
-      <c r="P3" s="16">
-        <v>0</v>
-      </c>
-      <c r="Q3" s="16">
-        <v>0</v>
-      </c>
-      <c r="R3" s="16">
-        <v>0</v>
-      </c>
-      <c r="S3" s="16">
-        <v>0</v>
-      </c>
-      <c r="T3" s="16">
-        <v>1</v>
-      </c>
-      <c r="U3" s="16">
-        <v>1</v>
-      </c>
-      <c r="V3" s="16">
-        <v>0</v>
-      </c>
-      <c r="W3" s="16">
-        <v>1</v>
-      </c>
-      <c r="X3" s="16">
-        <v>0</v>
-      </c>
-      <c r="Y3" s="16">
-        <v>1</v>
-      </c>
-      <c r="Z3" s="16">
-        <v>0</v>
-      </c>
-      <c r="AA3" s="16">
-        <v>1</v>
-      </c>
-      <c r="AB3" s="16">
+    <row r="2" spans="1:28" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="15">
+        <v>1</v>
+      </c>
+      <c r="B2" s="15">
+        <v>1</v>
+      </c>
+      <c r="C2" s="15">
+        <v>1</v>
+      </c>
+      <c r="D2" s="15">
+        <v>1</v>
+      </c>
+      <c r="E2" s="15">
+        <v>1</v>
+      </c>
+      <c r="F2" s="15">
+        <v>1</v>
+      </c>
+      <c r="G2" s="15">
+        <v>1</v>
+      </c>
+      <c r="H2" s="15">
+        <v>1</v>
+      </c>
+      <c r="I2" s="15">
+        <v>1</v>
+      </c>
+      <c r="J2" s="15">
+        <v>1</v>
+      </c>
+      <c r="K2" s="15">
+        <v>1</v>
+      </c>
+      <c r="L2" s="15">
+        <v>1</v>
+      </c>
+      <c r="M2" s="15">
+        <v>1</v>
+      </c>
+      <c r="N2" s="15">
+        <v>1</v>
+      </c>
+      <c r="O2" s="15">
+        <v>0</v>
+      </c>
+      <c r="P2" s="15">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="15">
+        <v>0</v>
+      </c>
+      <c r="R2" s="15">
+        <v>0</v>
+      </c>
+      <c r="S2" s="15">
+        <v>0</v>
+      </c>
+      <c r="T2" s="15">
+        <v>1</v>
+      </c>
+      <c r="U2" s="15">
+        <v>1</v>
+      </c>
+      <c r="V2" s="15">
+        <v>0</v>
+      </c>
+      <c r="W2" s="15">
+        <v>1</v>
+      </c>
+      <c r="X2" s="15">
+        <v>0</v>
+      </c>
+      <c r="Y2" s="15">
+        <v>1</v>
+      </c>
+      <c r="Z2" s="15">
+        <v>0</v>
+      </c>
+      <c r="AA2" s="15">
+        <v>1</v>
+      </c>
+      <c r="AB2" s="15">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update results, reorganize package
</commit_message>
<xml_diff>
--- a/dmsan/data/criteria_weight_scenarios.xlsx
+++ b/dmsan/data/criteria_weight_scenarios.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bfca01abaf64aab7/Coding/ds/dmsan/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{4C9980BB-C809-8949-A4CE-551CD5B3F79D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5DC71835-EC9B-314A-B4C3-8FC9DE93E694}"/>
+  <xr:revisionPtr revIDLastSave="18" documentId="13_ncr:1_{4C9980BB-C809-8949-A4CE-551CD5B3F79D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6C25473D-9A5D-E548-AFB0-838C6633CB0B}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15940" xr2:uid="{E854125C-2344-44F6-A254-41B8AFA7B554}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15940" activeTab="1" xr2:uid="{E854125C-2344-44F6-A254-41B8AFA7B554}"/>
   </bookViews>
   <sheets>
     <sheet name="definitions" sheetId="4" r:id="rId1"/>
     <sheet name="weight_scenarios" sheetId="3" r:id="rId2"/>
-    <sheet name="indicator_type" sheetId="6" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="230">
   <si>
     <t>LCA</t>
   </si>
@@ -732,7 +731,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -755,13 +754,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -833,7 +825,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -842,17 +834,11 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1172,8 +1158,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DAC3413-5145-4E90-ADD4-96F1E182146D}">
   <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1329,10 +1315,10 @@
       </c>
     </row>
     <row r="7" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="16" t="s">
+      <c r="A7" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="16" t="s">
+      <c r="B7" s="14" t="s">
         <v>40</v>
       </c>
       <c r="C7" s="3" t="s">
@@ -1353,83 +1339,83 @@
       </c>
     </row>
     <row r="8" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="16" t="s">
+      <c r="A8" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="16" t="s">
+      <c r="B8" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="D8" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="E8" s="10" t="s">
+      <c r="E8" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="F8" s="10" t="s">
+      <c r="F8" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="G8" s="10">
+      <c r="G8" s="9">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="16" t="s">
+      <c r="A9" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="16" t="s">
+      <c r="B9" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="C9" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="D9" s="10" t="s">
+      <c r="D9" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="E9" s="10" t="s">
+      <c r="E9" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="F9" s="10" t="s">
+      <c r="F9" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="G9" s="10">
+      <c r="G9" s="9">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H9" s="10"/>
+      <c r="H9" s="9"/>
     </row>
     <row r="10" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="16" t="s">
+      <c r="A10" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="16" t="s">
+      <c r="B10" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="C10" s="10" t="s">
+      <c r="C10" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="D10" s="10" t="s">
+      <c r="D10" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="E10" s="10" t="s">
+      <c r="E10" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="F10" s="10" t="s">
+      <c r="F10" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="G10" s="10">
+      <c r="G10" s="9">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="17" t="s">
+      <c r="A11" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="B11" s="17" t="s">
+      <c r="B11" s="15" t="s">
         <v>28</v>
       </c>
       <c r="C11" s="4" t="s">
@@ -1450,10 +1436,10 @@
       </c>
     </row>
     <row r="12" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="17" t="s">
+      <c r="A12" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="B12" s="17" t="s">
+      <c r="B12" s="15" t="s">
         <v>28</v>
       </c>
       <c r="C12" s="4" t="s">
@@ -1474,10 +1460,10 @@
       </c>
     </row>
     <row r="13" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="17" t="s">
+      <c r="A13" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="B13" s="17" t="s">
+      <c r="B13" s="15" t="s">
         <v>28</v>
       </c>
       <c r="C13" s="4" t="s">
@@ -1498,10 +1484,10 @@
       </c>
     </row>
     <row r="14" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="17" t="s">
+      <c r="A14" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="B14" s="17" t="s">
+      <c r="B14" s="15" t="s">
         <v>28</v>
       </c>
       <c r="C14" s="4" t="s">
@@ -1522,10 +1508,10 @@
       </c>
     </row>
     <row r="15" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="17" t="s">
+      <c r="A15" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="B15" s="17" t="s">
+      <c r="B15" s="15" t="s">
         <v>28</v>
       </c>
       <c r="C15" s="4" t="s">
@@ -1546,10 +1532,10 @@
       </c>
     </row>
     <row r="16" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="17" t="s">
+      <c r="A16" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="B16" s="17" t="s">
+      <c r="B16" s="15" t="s">
         <v>28</v>
       </c>
       <c r="C16" s="4" t="s">
@@ -1585,14 +1571,14 @@
       <c r="E17" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="F17" s="11" t="s">
+      <c r="F17" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="G17" s="11">
+      <c r="G17" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H17" s="11"/>
+      <c r="H17" s="10"/>
     </row>
     <row r="18" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
@@ -1610,14 +1596,14 @@
       <c r="E18" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="F18" s="11" t="s">
+      <c r="F18" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="G18" s="11">
+      <c r="G18" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H18" s="11"/>
+      <c r="H18" s="10"/>
     </row>
     <row r="19" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
@@ -1635,14 +1621,14 @@
       <c r="E19" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="F19" s="11" t="s">
+      <c r="F19" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="G19" s="11">
+      <c r="G19" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H19" s="11"/>
+      <c r="H19" s="10"/>
     </row>
     <row r="20" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="6" t="s">
@@ -1684,10 +1670,10 @@
       <c r="E21" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="F21" s="12" t="s">
+      <c r="F21" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="G21" s="12">
+      <c r="G21" s="11">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -1708,10 +1694,10 @@
       <c r="E22" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="F22" s="12" t="s">
+      <c r="F22" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="G22" s="12">
+      <c r="G22" s="11">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -1732,10 +1718,10 @@
       <c r="E23" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="F23" s="12" t="s">
+      <c r="F23" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="G23" s="12">
+      <c r="G23" s="11">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1756,10 +1742,10 @@
       <c r="E24" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="F24" s="12" t="s">
+      <c r="F24" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="G24" s="12">
+      <c r="G24" s="11">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -1780,10 +1766,10 @@
       <c r="E25" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="F25" s="12" t="s">
+      <c r="F25" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="G25" s="12">
+      <c r="G25" s="11">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1804,10 +1790,10 @@
       <c r="E26" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="F26" s="12" t="s">
+      <c r="F26" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="G26" s="12">
+      <c r="G26" s="11">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -1828,10 +1814,10 @@
       <c r="E27" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="F27" s="12" t="s">
+      <c r="F27" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="G27" s="12">
+      <c r="G27" s="11">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1852,10 +1838,10 @@
       <c r="E28" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="F28" s="12" t="s">
+      <c r="F28" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="G28" s="12">
+      <c r="G28" s="11">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -1876,18 +1862,18 @@
       <c r="E29" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="F29" s="12" t="s">
+      <c r="F29" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="G29" s="12">
+      <c r="G29" s="11">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D30" s="1"/>
-      <c r="F30" s="13"/>
-      <c r="G30" s="13"/>
+      <c r="F30" s="12"/>
+      <c r="G30" s="12"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D31" s="1"/>
@@ -1909,8 +1895,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6956783-CD8A-4021-B812-DCE07115A14C}">
   <dimension ref="A1:I53"/>
   <sheetViews>
-    <sheetView zoomScale="97" zoomScaleNormal="97" workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+    <sheetView tabSelected="1" zoomScale="97" zoomScaleNormal="97" workbookViewId="0">
+      <selection activeCell="I33" sqref="I33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1944,7 +1930,7 @@
       <c r="H1" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="I1" s="15" t="s">
+      <c r="I1" s="13" t="s">
         <v>107</v>
       </c>
     </row>
@@ -1952,25 +1938,25 @@
       <c r="A2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="C2" s="9">
-        <v>0.2</v>
-      </c>
-      <c r="D2" s="9">
-        <v>0</v>
-      </c>
-      <c r="E2" s="9">
-        <v>0</v>
-      </c>
-      <c r="F2" s="9">
-        <v>0</v>
-      </c>
-      <c r="G2" s="9">
-        <v>0</v>
-      </c>
-      <c r="H2" s="9">
+      <c r="C2" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="D2" s="8">
+        <v>0</v>
+      </c>
+      <c r="E2" s="8">
+        <v>0</v>
+      </c>
+      <c r="F2" s="8">
+        <v>0</v>
+      </c>
+      <c r="G2" s="8">
+        <v>0</v>
+      </c>
+      <c r="H2" s="8">
         <v>1</v>
       </c>
       <c r="I2" s="1" t="s">
@@ -1981,25 +1967,25 @@
       <c r="A3" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="C3" s="9">
-        <v>0</v>
-      </c>
-      <c r="D3" s="9">
-        <v>0.2</v>
-      </c>
-      <c r="E3" s="9">
-        <v>0</v>
-      </c>
-      <c r="F3" s="9">
-        <v>0</v>
-      </c>
-      <c r="G3" s="9">
-        <v>0</v>
-      </c>
-      <c r="H3" s="9">
+      <c r="C3" s="8">
+        <v>0</v>
+      </c>
+      <c r="D3" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="E3" s="8">
+        <v>0</v>
+      </c>
+      <c r="F3" s="8">
+        <v>0</v>
+      </c>
+      <c r="G3" s="8">
+        <v>0</v>
+      </c>
+      <c r="H3" s="8">
         <v>1</v>
       </c>
       <c r="I3" s="1" t="s">
@@ -2010,25 +1996,25 @@
       <c r="A4" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="C4" s="9">
-        <v>0</v>
-      </c>
-      <c r="D4" s="9">
-        <v>0</v>
-      </c>
-      <c r="E4" s="9">
-        <v>0.2</v>
-      </c>
-      <c r="F4" s="9">
-        <v>0</v>
-      </c>
-      <c r="G4" s="9">
-        <v>0</v>
-      </c>
-      <c r="H4" s="9">
+      <c r="C4" s="8">
+        <v>0</v>
+      </c>
+      <c r="D4" s="8">
+        <v>0</v>
+      </c>
+      <c r="E4" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="F4" s="8">
+        <v>0</v>
+      </c>
+      <c r="G4" s="8">
+        <v>0</v>
+      </c>
+      <c r="H4" s="8">
         <v>1</v>
       </c>
       <c r="I4" s="1" t="s">
@@ -2039,25 +2025,25 @@
       <c r="A5" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="C5" s="9">
-        <v>0</v>
-      </c>
-      <c r="D5" s="9">
-        <v>0</v>
-      </c>
-      <c r="E5" s="9">
-        <v>0</v>
-      </c>
-      <c r="F5" s="9">
-        <v>0.2</v>
-      </c>
-      <c r="G5" s="9">
-        <v>0</v>
-      </c>
-      <c r="H5" s="9">
+      <c r="C5" s="8">
+        <v>0</v>
+      </c>
+      <c r="D5" s="8">
+        <v>0</v>
+      </c>
+      <c r="E5" s="8">
+        <v>0</v>
+      </c>
+      <c r="F5" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="G5" s="8">
+        <v>0</v>
+      </c>
+      <c r="H5" s="8">
         <v>1</v>
       </c>
       <c r="I5" s="1" t="s">
@@ -2068,25 +2054,25 @@
       <c r="A6" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="C6" s="9">
-        <v>0</v>
-      </c>
-      <c r="D6" s="9">
-        <v>0</v>
-      </c>
-      <c r="E6" s="9">
-        <v>0</v>
-      </c>
-      <c r="F6" s="9">
-        <v>0</v>
-      </c>
-      <c r="G6" s="9">
-        <v>0.2</v>
-      </c>
-      <c r="H6" s="9">
+      <c r="C6" s="8">
+        <v>0</v>
+      </c>
+      <c r="D6" s="8">
+        <v>0</v>
+      </c>
+      <c r="E6" s="8">
+        <v>0</v>
+      </c>
+      <c r="F6" s="8">
+        <v>0</v>
+      </c>
+      <c r="G6" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="H6" s="8">
         <v>1</v>
       </c>
       <c r="I6" s="1" t="s">
@@ -2097,25 +2083,25 @@
       <c r="A7" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="9">
-        <v>0.2</v>
-      </c>
-      <c r="D7" s="9">
-        <v>0.2</v>
-      </c>
-      <c r="E7" s="9">
-        <v>0.2</v>
-      </c>
-      <c r="F7" s="9">
-        <v>0.2</v>
-      </c>
-      <c r="G7" s="9">
-        <v>0.2</v>
-      </c>
-      <c r="H7" s="9">
+      <c r="C7" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="D7" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="E7" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="F7" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="G7" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="H7" s="8">
         <v>5</v>
       </c>
       <c r="I7" s="1" t="s">
@@ -2126,25 +2112,25 @@
       <c r="A8" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="C8" s="9">
-        <v>0.2</v>
-      </c>
-      <c r="D8" s="9">
-        <v>0.2</v>
-      </c>
-      <c r="E8" s="9">
-        <v>0</v>
-      </c>
-      <c r="F8" s="9">
-        <v>0</v>
-      </c>
-      <c r="G8" s="9">
-        <v>0</v>
-      </c>
-      <c r="H8" s="9">
+      <c r="C8" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="D8" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="E8" s="8">
+        <v>0</v>
+      </c>
+      <c r="F8" s="8">
+        <v>0</v>
+      </c>
+      <c r="G8" s="8">
+        <v>0</v>
+      </c>
+      <c r="H8" s="8">
         <v>2</v>
       </c>
       <c r="I8" s="1" t="s">
@@ -2155,25 +2141,25 @@
       <c r="A9" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="8" t="s">
         <v>157</v>
       </c>
-      <c r="C9" s="9">
-        <v>0.2</v>
-      </c>
-      <c r="D9" s="9">
-        <v>0.2</v>
-      </c>
-      <c r="E9" s="9">
-        <v>0.2</v>
-      </c>
-      <c r="F9" s="9">
-        <v>0</v>
-      </c>
-      <c r="G9" s="9">
-        <v>0</v>
-      </c>
-      <c r="H9" s="9">
+      <c r="C9" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="D9" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="E9" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="F9" s="8">
+        <v>0</v>
+      </c>
+      <c r="G9" s="8">
+        <v>0</v>
+      </c>
+      <c r="H9" s="8">
         <v>3</v>
       </c>
       <c r="I9" s="1" t="s">
@@ -2184,25 +2170,25 @@
       <c r="A10" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="8" t="s">
         <v>163</v>
       </c>
-      <c r="C10" s="9">
-        <v>0.2</v>
-      </c>
-      <c r="D10" s="9">
-        <v>0.2</v>
-      </c>
-      <c r="E10" s="9">
-        <v>0.2</v>
-      </c>
-      <c r="F10" s="9">
-        <v>0.2</v>
-      </c>
-      <c r="G10" s="9">
-        <v>0</v>
-      </c>
-      <c r="H10" s="9">
+      <c r="C10" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="D10" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="E10" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="F10" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="G10" s="8">
+        <v>0</v>
+      </c>
+      <c r="H10" s="8">
         <v>4</v>
       </c>
       <c r="I10" s="1" t="s">
@@ -2213,25 +2199,25 @@
       <c r="A11" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="B11" s="9" t="s">
+      <c r="B11" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="C11" s="9">
-        <v>0.2</v>
-      </c>
-      <c r="D11" s="9">
-        <v>0</v>
-      </c>
-      <c r="E11" s="9">
-        <v>0.2</v>
-      </c>
-      <c r="F11" s="9">
-        <v>0</v>
-      </c>
-      <c r="G11" s="9">
-        <v>0</v>
-      </c>
-      <c r="H11" s="9">
+      <c r="C11" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="D11" s="8">
+        <v>0</v>
+      </c>
+      <c r="E11" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="F11" s="8">
+        <v>0</v>
+      </c>
+      <c r="G11" s="8">
+        <v>0</v>
+      </c>
+      <c r="H11" s="8">
         <v>2</v>
       </c>
       <c r="I11" s="1" t="s">
@@ -2242,25 +2228,25 @@
       <c r="A12" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="B12" s="9" t="s">
+      <c r="B12" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="C12" s="9">
-        <v>0.2</v>
-      </c>
-      <c r="D12" s="9">
-        <v>0</v>
-      </c>
-      <c r="E12" s="9">
-        <v>0</v>
-      </c>
-      <c r="F12" s="9">
-        <v>0.2</v>
-      </c>
-      <c r="G12" s="9">
-        <v>0</v>
-      </c>
-      <c r="H12" s="9">
+      <c r="C12" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="D12" s="8">
+        <v>0</v>
+      </c>
+      <c r="E12" s="8">
+        <v>0</v>
+      </c>
+      <c r="F12" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="G12" s="8">
+        <v>0</v>
+      </c>
+      <c r="H12" s="8">
         <v>2</v>
       </c>
       <c r="I12" s="1" t="s">
@@ -2271,25 +2257,25 @@
       <c r="A13" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="B13" s="9" t="s">
+      <c r="B13" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="C13" s="9">
-        <v>0.2</v>
-      </c>
-      <c r="D13" s="9">
-        <v>0</v>
-      </c>
-      <c r="E13" s="9">
-        <v>0</v>
-      </c>
-      <c r="F13" s="9">
-        <v>0</v>
-      </c>
-      <c r="G13" s="9">
-        <v>0.2</v>
-      </c>
-      <c r="H13" s="9">
+      <c r="C13" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="D13" s="8">
+        <v>0</v>
+      </c>
+      <c r="E13" s="8">
+        <v>0</v>
+      </c>
+      <c r="F13" s="8">
+        <v>0</v>
+      </c>
+      <c r="G13" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="H13" s="8">
         <v>2</v>
       </c>
       <c r="I13" s="1" t="s">
@@ -2300,25 +2286,25 @@
       <c r="A14" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="B14" s="9" t="s">
+      <c r="B14" s="8" t="s">
         <v>157</v>
       </c>
-      <c r="C14" s="9">
-        <v>0.2</v>
-      </c>
-      <c r="D14" s="9">
-        <v>0.2</v>
-      </c>
-      <c r="E14" s="9">
-        <v>0.2</v>
-      </c>
-      <c r="F14" s="9">
-        <v>0</v>
-      </c>
-      <c r="G14" s="9">
-        <v>0</v>
-      </c>
-      <c r="H14" s="9">
+      <c r="C14" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="D14" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="E14" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="F14" s="8">
+        <v>0</v>
+      </c>
+      <c r="G14" s="8">
+        <v>0</v>
+      </c>
+      <c r="H14" s="8">
         <v>3</v>
       </c>
       <c r="I14" s="1" t="s">
@@ -2329,25 +2315,25 @@
       <c r="A15" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="B15" s="9" t="s">
+      <c r="B15" s="8" t="s">
         <v>163</v>
       </c>
-      <c r="C15" s="9">
-        <v>0.2</v>
-      </c>
-      <c r="D15" s="9">
-        <v>0.2</v>
-      </c>
-      <c r="E15" s="9">
-        <v>0.2</v>
-      </c>
-      <c r="F15" s="9">
-        <v>0.2</v>
-      </c>
-      <c r="G15" s="9">
-        <v>0</v>
-      </c>
-      <c r="H15" s="9">
+      <c r="C15" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="D15" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="E15" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="F15" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="G15" s="8">
+        <v>0</v>
+      </c>
+      <c r="H15" s="8">
         <v>4</v>
       </c>
       <c r="I15" s="1" t="s">
@@ -2358,25 +2344,25 @@
       <c r="A16" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="B16" s="9" t="s">
+      <c r="B16" s="8" t="s">
         <v>164</v>
       </c>
-      <c r="C16" s="9">
-        <v>0.2</v>
-      </c>
-      <c r="D16" s="9">
-        <v>0</v>
-      </c>
-      <c r="E16" s="9">
-        <v>0.2</v>
-      </c>
-      <c r="F16" s="9">
-        <v>0.2</v>
-      </c>
-      <c r="G16" s="9">
-        <v>0.2</v>
-      </c>
-      <c r="H16" s="9">
+      <c r="C16" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="D16" s="8">
+        <v>0</v>
+      </c>
+      <c r="E16" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="F16" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="G16" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="H16" s="8">
         <v>4</v>
       </c>
       <c r="I16" s="1" t="s">
@@ -2387,25 +2373,25 @@
       <c r="A17" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="B17" s="9" t="s">
+      <c r="B17" s="8" t="s">
         <v>158</v>
       </c>
-      <c r="C17" s="9">
-        <v>0.2</v>
-      </c>
-      <c r="D17" s="9">
-        <v>0</v>
-      </c>
-      <c r="E17" s="9">
-        <v>0.2</v>
-      </c>
-      <c r="F17" s="9">
-        <v>0</v>
-      </c>
-      <c r="G17" s="9">
-        <v>0.2</v>
-      </c>
-      <c r="H17" s="9">
+      <c r="C17" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="D17" s="8">
+        <v>0</v>
+      </c>
+      <c r="E17" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="F17" s="8">
+        <v>0</v>
+      </c>
+      <c r="G17" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="H17" s="8">
         <v>3</v>
       </c>
       <c r="I17" s="1" t="s">
@@ -2416,25 +2402,25 @@
       <c r="A18" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="B18" s="9" t="s">
+      <c r="B18" s="8" t="s">
         <v>165</v>
       </c>
-      <c r="C18" s="9">
-        <v>0</v>
-      </c>
-      <c r="D18" s="9">
-        <v>0.2</v>
-      </c>
-      <c r="E18" s="9">
-        <v>0.2</v>
-      </c>
-      <c r="F18" s="9">
-        <v>0.2</v>
-      </c>
-      <c r="G18" s="9">
-        <v>0.2</v>
-      </c>
-      <c r="H18" s="9">
+      <c r="C18" s="8">
+        <v>0</v>
+      </c>
+      <c r="D18" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="E18" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="F18" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="G18" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="H18" s="8">
         <v>4</v>
       </c>
       <c r="I18" s="1" t="s">
@@ -2445,25 +2431,25 @@
       <c r="A19" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="B19" s="9" t="s">
+      <c r="B19" s="8" t="s">
         <v>162</v>
       </c>
-      <c r="C19" s="9">
-        <v>0</v>
-      </c>
-      <c r="D19" s="9">
-        <v>0</v>
-      </c>
-      <c r="E19" s="9">
-        <v>0.2</v>
-      </c>
-      <c r="F19" s="9">
-        <v>0.2</v>
-      </c>
-      <c r="G19" s="9">
-        <v>0.2</v>
-      </c>
-      <c r="H19" s="9">
+      <c r="C19" s="8">
+        <v>0</v>
+      </c>
+      <c r="D19" s="8">
+        <v>0</v>
+      </c>
+      <c r="E19" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="F19" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="G19" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="H19" s="8">
         <v>3</v>
       </c>
       <c r="I19" s="1" t="s">
@@ -2474,25 +2460,25 @@
       <c r="A20" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="B20" s="9" t="s">
+      <c r="B20" s="8" t="s">
         <v>156</v>
       </c>
-      <c r="C20" s="9">
-        <v>0</v>
-      </c>
-      <c r="D20" s="9">
-        <v>0</v>
-      </c>
-      <c r="E20" s="9">
-        <v>0</v>
-      </c>
-      <c r="F20" s="9">
-        <v>0.2</v>
-      </c>
-      <c r="G20" s="9">
-        <v>0.2</v>
-      </c>
-      <c r="H20" s="9">
+      <c r="C20" s="8">
+        <v>0</v>
+      </c>
+      <c r="D20" s="8">
+        <v>0</v>
+      </c>
+      <c r="E20" s="8">
+        <v>0</v>
+      </c>
+      <c r="F20" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="G20" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="H20" s="8">
         <v>2</v>
       </c>
       <c r="I20" s="1" t="s">
@@ -2503,25 +2489,25 @@
       <c r="A21" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="B21" s="9" t="s">
+      <c r="B21" s="8" t="s">
         <v>160</v>
       </c>
-      <c r="C21" s="9">
-        <v>0</v>
-      </c>
-      <c r="D21" s="9">
-        <v>0.2</v>
-      </c>
-      <c r="E21" s="9">
-        <v>0.2</v>
-      </c>
-      <c r="F21" s="9">
-        <v>0</v>
-      </c>
-      <c r="G21" s="9">
-        <v>0.2</v>
-      </c>
-      <c r="H21" s="9">
+      <c r="C21" s="8">
+        <v>0</v>
+      </c>
+      <c r="D21" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="E21" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="F21" s="8">
+        <v>0</v>
+      </c>
+      <c r="G21" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="H21" s="8">
         <v>3</v>
       </c>
       <c r="I21" s="1" t="s">
@@ -2532,25 +2518,25 @@
       <c r="A22" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="B22" s="9" t="s">
+      <c r="B22" s="8" t="s">
         <v>152</v>
       </c>
-      <c r="C22" s="9">
-        <v>0</v>
-      </c>
-      <c r="D22" s="9">
-        <v>0.2</v>
-      </c>
-      <c r="E22" s="9">
-        <v>0.2</v>
-      </c>
-      <c r="F22" s="9">
-        <v>0</v>
-      </c>
-      <c r="G22" s="9">
-        <v>0</v>
-      </c>
-      <c r="H22" s="9">
+      <c r="C22" s="8">
+        <v>0</v>
+      </c>
+      <c r="D22" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="E22" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="F22" s="8">
+        <v>0</v>
+      </c>
+      <c r="G22" s="8">
+        <v>0</v>
+      </c>
+      <c r="H22" s="8">
         <v>2</v>
       </c>
       <c r="I22" s="1" t="s">
@@ -2561,25 +2547,25 @@
       <c r="A23" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="B23" s="9" t="s">
+      <c r="B23" s="8" t="s">
         <v>155</v>
       </c>
-      <c r="C23" s="9">
-        <v>0</v>
-      </c>
-      <c r="D23" s="9">
-        <v>0</v>
-      </c>
-      <c r="E23" s="9">
-        <v>0.2</v>
-      </c>
-      <c r="F23" s="9">
-        <v>0</v>
-      </c>
-      <c r="G23" s="9">
-        <v>0.2</v>
-      </c>
-      <c r="H23" s="9">
+      <c r="C23" s="8">
+        <v>0</v>
+      </c>
+      <c r="D23" s="8">
+        <v>0</v>
+      </c>
+      <c r="E23" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="F23" s="8">
+        <v>0</v>
+      </c>
+      <c r="G23" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="H23" s="8">
         <v>2</v>
       </c>
       <c r="I23" s="1" t="s">
@@ -2590,25 +2576,25 @@
       <c r="A24" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="B24" s="9" t="s">
+      <c r="B24" s="8" t="s">
         <v>154</v>
       </c>
-      <c r="C24" s="9">
-        <v>0</v>
-      </c>
-      <c r="D24" s="9">
-        <v>0</v>
-      </c>
-      <c r="E24" s="9">
-        <v>0.2</v>
-      </c>
-      <c r="F24" s="9">
-        <v>0.2</v>
-      </c>
-      <c r="G24" s="9">
-        <v>0</v>
-      </c>
-      <c r="H24" s="9">
+      <c r="C24" s="8">
+        <v>0</v>
+      </c>
+      <c r="D24" s="8">
+        <v>0</v>
+      </c>
+      <c r="E24" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="F24" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="G24" s="8">
+        <v>0</v>
+      </c>
+      <c r="H24" s="8">
         <v>2</v>
       </c>
       <c r="I24" s="1" t="s">
@@ -2619,25 +2605,25 @@
       <c r="A25" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="B25" s="9" t="s">
+      <c r="B25" s="8" t="s">
         <v>161</v>
       </c>
-      <c r="C25" s="9">
-        <v>0</v>
-      </c>
-      <c r="D25" s="9">
-        <v>0.2</v>
-      </c>
-      <c r="E25" s="9">
-        <v>0</v>
-      </c>
-      <c r="F25" s="9">
-        <v>0.2</v>
-      </c>
-      <c r="G25" s="9">
-        <v>0.2</v>
-      </c>
-      <c r="H25" s="9">
+      <c r="C25" s="8">
+        <v>0</v>
+      </c>
+      <c r="D25" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="E25" s="8">
+        <v>0</v>
+      </c>
+      <c r="F25" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="G25" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="H25" s="8">
         <v>3</v>
       </c>
       <c r="I25" s="1" t="s">
@@ -2648,25 +2634,25 @@
       <c r="A26" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="B26" s="9" t="s">
+      <c r="B26" s="8" t="s">
         <v>153</v>
       </c>
-      <c r="C26" s="9">
-        <v>0</v>
-      </c>
-      <c r="D26" s="9">
-        <v>0.2</v>
-      </c>
-      <c r="E26" s="9">
-        <v>0</v>
-      </c>
-      <c r="F26" s="9">
-        <v>0.2</v>
-      </c>
-      <c r="G26" s="9">
-        <v>0</v>
-      </c>
-      <c r="H26" s="9">
+      <c r="C26" s="8">
+        <v>0</v>
+      </c>
+      <c r="D26" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="E26" s="8">
+        <v>0</v>
+      </c>
+      <c r="F26" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="G26" s="8">
+        <v>0</v>
+      </c>
+      <c r="H26" s="8">
         <v>2</v>
       </c>
       <c r="I26" s="1" t="s">
@@ -2677,25 +2663,25 @@
       <c r="A27" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="B27" s="9" t="s">
+      <c r="B27" s="8" t="s">
         <v>159</v>
       </c>
-      <c r="C27" s="9">
-        <v>0</v>
-      </c>
-      <c r="D27" s="9">
-        <v>0.2</v>
-      </c>
-      <c r="E27" s="9">
-        <v>0.2</v>
-      </c>
-      <c r="F27" s="9">
-        <v>0.2</v>
-      </c>
-      <c r="G27" s="9">
-        <v>0</v>
-      </c>
-      <c r="H27" s="9">
+      <c r="C27" s="8">
+        <v>0</v>
+      </c>
+      <c r="D27" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="E27" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="F27" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="G27" s="8">
+        <v>0</v>
+      </c>
+      <c r="H27" s="8">
         <v>3</v>
       </c>
       <c r="I27" s="1" t="s">
@@ -2706,25 +2692,25 @@
       <c r="A28" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="B28" s="9" t="s">
+      <c r="B28" s="8" t="s">
         <v>168</v>
       </c>
-      <c r="C28" s="9">
+      <c r="C28" s="8">
         <v>0.4</v>
       </c>
-      <c r="D28" s="9">
-        <v>0.2</v>
-      </c>
-      <c r="E28" s="9">
-        <v>0</v>
-      </c>
-      <c r="F28" s="9">
-        <v>0</v>
-      </c>
-      <c r="G28" s="9">
-        <v>0</v>
-      </c>
-      <c r="H28" s="9">
+      <c r="D28" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="E28" s="8">
+        <v>0</v>
+      </c>
+      <c r="F28" s="8">
+        <v>0</v>
+      </c>
+      <c r="G28" s="8">
+        <v>0</v>
+      </c>
+      <c r="H28" s="8">
         <v>2</v>
       </c>
       <c r="I28" s="1" t="s">
@@ -2735,25 +2721,25 @@
       <c r="A29" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="B29" s="9" t="s">
+      <c r="B29" s="8" t="s">
         <v>170</v>
       </c>
-      <c r="C29" s="9">
+      <c r="C29" s="8">
         <v>0.4</v>
       </c>
-      <c r="D29" s="9">
-        <v>0</v>
-      </c>
-      <c r="E29" s="9">
-        <v>0.2</v>
-      </c>
-      <c r="F29" s="9">
-        <v>0</v>
-      </c>
-      <c r="G29" s="9">
-        <v>0</v>
-      </c>
-      <c r="H29" s="9">
+      <c r="D29" s="8">
+        <v>0</v>
+      </c>
+      <c r="E29" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="F29" s="8">
+        <v>0</v>
+      </c>
+      <c r="G29" s="8">
+        <v>0</v>
+      </c>
+      <c r="H29" s="8">
         <v>2</v>
       </c>
       <c r="I29" s="1" t="s">
@@ -2764,25 +2750,25 @@
       <c r="A30" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="B30" s="9" t="s">
+      <c r="B30" s="8" t="s">
         <v>172</v>
       </c>
-      <c r="C30" s="9">
+      <c r="C30" s="8">
         <v>0.4</v>
       </c>
-      <c r="D30" s="9">
-        <v>0</v>
-      </c>
-      <c r="E30" s="9">
-        <v>0</v>
-      </c>
-      <c r="F30" s="9">
-        <v>0.2</v>
-      </c>
-      <c r="G30" s="9">
-        <v>0</v>
-      </c>
-      <c r="H30" s="9">
+      <c r="D30" s="8">
+        <v>0</v>
+      </c>
+      <c r="E30" s="8">
+        <v>0</v>
+      </c>
+      <c r="F30" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="G30" s="8">
+        <v>0</v>
+      </c>
+      <c r="H30" s="8">
         <v>2</v>
       </c>
       <c r="I30" s="1" t="s">
@@ -2793,25 +2779,25 @@
       <c r="A31" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="B31" s="9" t="s">
+      <c r="B31" s="8" t="s">
         <v>174</v>
       </c>
-      <c r="C31" s="9">
+      <c r="C31" s="8">
         <v>0.4</v>
       </c>
-      <c r="D31" s="9">
-        <v>0</v>
-      </c>
-      <c r="E31" s="9">
-        <v>0</v>
-      </c>
-      <c r="F31" s="9">
-        <v>0</v>
-      </c>
-      <c r="G31" s="9">
-        <v>0.2</v>
-      </c>
-      <c r="H31" s="9">
+      <c r="D31" s="8">
+        <v>0</v>
+      </c>
+      <c r="E31" s="8">
+        <v>0</v>
+      </c>
+      <c r="F31" s="8">
+        <v>0</v>
+      </c>
+      <c r="G31" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="H31" s="8">
         <v>2</v>
       </c>
       <c r="I31" s="1" t="s">
@@ -2822,25 +2808,25 @@
       <c r="A32" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="B32" s="9" t="s">
+      <c r="B32" s="8" t="s">
         <v>176</v>
       </c>
-      <c r="C32" s="9">
-        <v>0.2</v>
-      </c>
-      <c r="D32" s="9">
+      <c r="C32" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="D32" s="8">
         <v>0.4</v>
       </c>
-      <c r="E32" s="9">
-        <v>0</v>
-      </c>
-      <c r="F32" s="9">
-        <v>0</v>
-      </c>
-      <c r="G32" s="9">
-        <v>0</v>
-      </c>
-      <c r="H32" s="9">
+      <c r="E32" s="8">
+        <v>0</v>
+      </c>
+      <c r="F32" s="8">
+        <v>0</v>
+      </c>
+      <c r="G32" s="8">
+        <v>0</v>
+      </c>
+      <c r="H32" s="8">
         <v>2</v>
       </c>
       <c r="I32" s="1" t="s">
@@ -2851,25 +2837,25 @@
       <c r="A33" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="B33" s="9" t="s">
+      <c r="B33" s="8" t="s">
         <v>178</v>
       </c>
-      <c r="C33" s="9">
-        <v>0</v>
-      </c>
-      <c r="D33" s="9">
+      <c r="C33" s="8">
+        <v>0</v>
+      </c>
+      <c r="D33" s="8">
         <v>0.4</v>
       </c>
-      <c r="E33" s="9">
-        <v>0.2</v>
-      </c>
-      <c r="F33" s="9">
-        <v>0</v>
-      </c>
-      <c r="G33" s="9">
-        <v>0</v>
-      </c>
-      <c r="H33" s="9">
+      <c r="E33" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="F33" s="8">
+        <v>0</v>
+      </c>
+      <c r="G33" s="8">
+        <v>0</v>
+      </c>
+      <c r="H33" s="8">
         <v>2</v>
       </c>
       <c r="I33" s="1" t="s">
@@ -2880,25 +2866,25 @@
       <c r="A34" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="B34" s="9" t="s">
+      <c r="B34" s="8" t="s">
         <v>180</v>
       </c>
-      <c r="C34" s="9">
-        <v>0</v>
-      </c>
-      <c r="D34" s="9">
+      <c r="C34" s="8">
+        <v>0</v>
+      </c>
+      <c r="D34" s="8">
         <v>0.4</v>
       </c>
-      <c r="E34" s="9">
-        <v>0</v>
-      </c>
-      <c r="F34" s="9">
-        <v>0.2</v>
-      </c>
-      <c r="G34" s="9">
-        <v>0</v>
-      </c>
-      <c r="H34" s="9">
+      <c r="E34" s="8">
+        <v>0</v>
+      </c>
+      <c r="F34" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="G34" s="8">
+        <v>0</v>
+      </c>
+      <c r="H34" s="8">
         <v>2</v>
       </c>
       <c r="I34" s="1" t="s">
@@ -2909,25 +2895,25 @@
       <c r="A35" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="B35" s="9" t="s">
+      <c r="B35" s="8" t="s">
         <v>182</v>
       </c>
-      <c r="C35" s="9">
-        <v>0</v>
-      </c>
-      <c r="D35" s="9">
+      <c r="C35" s="8">
+        <v>0</v>
+      </c>
+      <c r="D35" s="8">
         <v>0.4</v>
       </c>
-      <c r="E35" s="9">
-        <v>0</v>
-      </c>
-      <c r="F35" s="9">
-        <v>0</v>
-      </c>
-      <c r="G35" s="9">
-        <v>0.2</v>
-      </c>
-      <c r="H35" s="9">
+      <c r="E35" s="8">
+        <v>0</v>
+      </c>
+      <c r="F35" s="8">
+        <v>0</v>
+      </c>
+      <c r="G35" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="H35" s="8">
         <v>2</v>
       </c>
       <c r="I35" s="1" t="s">
@@ -2938,25 +2924,25 @@
       <c r="A36" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="B36" s="9" t="s">
+      <c r="B36" s="8" t="s">
         <v>184</v>
       </c>
-      <c r="C36" s="9">
-        <v>0.2</v>
-      </c>
-      <c r="D36" s="9">
-        <v>0</v>
-      </c>
-      <c r="E36" s="9">
+      <c r="C36" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="D36" s="8">
+        <v>0</v>
+      </c>
+      <c r="E36" s="8">
         <v>0.4</v>
       </c>
-      <c r="F36" s="9">
-        <v>0</v>
-      </c>
-      <c r="G36" s="9">
-        <v>0</v>
-      </c>
-      <c r="H36" s="9">
+      <c r="F36" s="8">
+        <v>0</v>
+      </c>
+      <c r="G36" s="8">
+        <v>0</v>
+      </c>
+      <c r="H36" s="8">
         <v>2</v>
       </c>
       <c r="I36" s="1" t="s">
@@ -2967,25 +2953,25 @@
       <c r="A37" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="B37" s="9" t="s">
+      <c r="B37" s="8" t="s">
         <v>186</v>
       </c>
-      <c r="C37" s="9">
-        <v>0</v>
-      </c>
-      <c r="D37" s="9">
-        <v>0.2</v>
-      </c>
-      <c r="E37" s="9">
+      <c r="C37" s="8">
+        <v>0</v>
+      </c>
+      <c r="D37" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="E37" s="8">
         <v>0.4</v>
       </c>
-      <c r="F37" s="9">
-        <v>0</v>
-      </c>
-      <c r="G37" s="9">
-        <v>0</v>
-      </c>
-      <c r="H37" s="9">
+      <c r="F37" s="8">
+        <v>0</v>
+      </c>
+      <c r="G37" s="8">
+        <v>0</v>
+      </c>
+      <c r="H37" s="8">
         <v>2</v>
       </c>
       <c r="I37" s="1" t="s">
@@ -2996,25 +2982,25 @@
       <c r="A38" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="B38" s="9" t="s">
+      <c r="B38" s="8" t="s">
         <v>194</v>
       </c>
-      <c r="C38" s="9">
-        <v>0</v>
-      </c>
-      <c r="D38" s="9">
-        <v>0</v>
-      </c>
-      <c r="E38" s="9">
+      <c r="C38" s="8">
+        <v>0</v>
+      </c>
+      <c r="D38" s="8">
+        <v>0</v>
+      </c>
+      <c r="E38" s="8">
         <v>0.4</v>
       </c>
-      <c r="F38" s="9">
-        <v>0.2</v>
-      </c>
-      <c r="G38" s="9">
-        <v>0</v>
-      </c>
-      <c r="H38" s="9">
+      <c r="F38" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="G38" s="8">
+        <v>0</v>
+      </c>
+      <c r="H38" s="8">
         <v>2</v>
       </c>
       <c r="I38" s="1" t="s">
@@ -3025,25 +3011,25 @@
       <c r="A39" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="B39" s="9" t="s">
+      <c r="B39" s="8" t="s">
         <v>197</v>
       </c>
-      <c r="C39" s="9">
-        <v>0</v>
-      </c>
-      <c r="D39" s="9">
-        <v>0</v>
-      </c>
-      <c r="E39" s="9">
+      <c r="C39" s="8">
+        <v>0</v>
+      </c>
+      <c r="D39" s="8">
+        <v>0</v>
+      </c>
+      <c r="E39" s="8">
         <v>0.4</v>
       </c>
-      <c r="F39" s="9">
-        <v>0</v>
-      </c>
-      <c r="G39" s="9">
-        <v>0.2</v>
-      </c>
-      <c r="H39" s="9">
+      <c r="F39" s="8">
+        <v>0</v>
+      </c>
+      <c r="G39" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="H39" s="8">
         <v>2</v>
       </c>
       <c r="I39" s="1" t="s">
@@ -3054,25 +3040,25 @@
       <c r="A40" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="B40" s="9" t="s">
+      <c r="B40" s="8" t="s">
         <v>199</v>
       </c>
-      <c r="C40" s="9">
-        <v>0.2</v>
-      </c>
-      <c r="D40" s="9">
-        <v>0</v>
-      </c>
-      <c r="E40" s="9">
-        <v>0</v>
-      </c>
-      <c r="F40" s="9">
+      <c r="C40" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="D40" s="8">
+        <v>0</v>
+      </c>
+      <c r="E40" s="8">
+        <v>0</v>
+      </c>
+      <c r="F40" s="8">
         <v>0.4</v>
       </c>
-      <c r="G40" s="9">
-        <v>0</v>
-      </c>
-      <c r="H40" s="9">
+      <c r="G40" s="8">
+        <v>0</v>
+      </c>
+      <c r="H40" s="8">
         <v>2</v>
       </c>
       <c r="I40" s="1" t="s">
@@ -3083,25 +3069,25 @@
       <c r="A41" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="B41" s="9" t="s">
+      <c r="B41" s="8" t="s">
         <v>201</v>
       </c>
-      <c r="C41" s="9">
-        <v>0</v>
-      </c>
-      <c r="D41" s="9">
-        <v>0.2</v>
-      </c>
-      <c r="E41" s="9">
-        <v>0</v>
-      </c>
-      <c r="F41" s="9">
+      <c r="C41" s="8">
+        <v>0</v>
+      </c>
+      <c r="D41" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="E41" s="8">
+        <v>0</v>
+      </c>
+      <c r="F41" s="8">
         <v>0.4</v>
       </c>
-      <c r="G41" s="9">
-        <v>0</v>
-      </c>
-      <c r="H41" s="9">
+      <c r="G41" s="8">
+        <v>0</v>
+      </c>
+      <c r="H41" s="8">
         <v>2</v>
       </c>
       <c r="I41" s="1" t="s">
@@ -3112,25 +3098,25 @@
       <c r="A42" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="B42" s="9" t="s">
+      <c r="B42" s="8" t="s">
         <v>203</v>
       </c>
-      <c r="C42" s="9">
-        <v>0</v>
-      </c>
-      <c r="D42" s="9">
-        <v>0</v>
-      </c>
-      <c r="E42" s="9">
-        <v>0.2</v>
-      </c>
-      <c r="F42" s="9">
+      <c r="C42" s="8">
+        <v>0</v>
+      </c>
+      <c r="D42" s="8">
+        <v>0</v>
+      </c>
+      <c r="E42" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="F42" s="8">
         <v>0.4</v>
       </c>
-      <c r="G42" s="9">
-        <v>0</v>
-      </c>
-      <c r="H42" s="9">
+      <c r="G42" s="8">
+        <v>0</v>
+      </c>
+      <c r="H42" s="8">
         <v>2</v>
       </c>
       <c r="I42" s="1" t="s">
@@ -3141,25 +3127,25 @@
       <c r="A43" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="B43" s="9" t="s">
+      <c r="B43" s="8" t="s">
         <v>205</v>
       </c>
-      <c r="C43" s="9">
-        <v>0</v>
-      </c>
-      <c r="D43" s="9">
-        <v>0</v>
-      </c>
-      <c r="E43" s="9">
-        <v>0</v>
-      </c>
-      <c r="F43" s="9">
+      <c r="C43" s="8">
+        <v>0</v>
+      </c>
+      <c r="D43" s="8">
+        <v>0</v>
+      </c>
+      <c r="E43" s="8">
+        <v>0</v>
+      </c>
+      <c r="F43" s="8">
         <v>0.4</v>
       </c>
-      <c r="G43" s="9">
-        <v>0.2</v>
-      </c>
-      <c r="H43" s="9">
+      <c r="G43" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="H43" s="8">
         <v>2</v>
       </c>
       <c r="I43" s="1" t="s">
@@ -3170,25 +3156,25 @@
       <c r="A44" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="B44" s="9" t="s">
+      <c r="B44" s="8" t="s">
         <v>207</v>
       </c>
-      <c r="C44" s="9">
-        <v>0.2</v>
-      </c>
-      <c r="D44" s="9">
-        <v>0</v>
-      </c>
-      <c r="E44" s="9">
-        <v>0</v>
-      </c>
-      <c r="F44" s="9">
-        <v>0</v>
-      </c>
-      <c r="G44" s="9">
+      <c r="C44" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="D44" s="8">
+        <v>0</v>
+      </c>
+      <c r="E44" s="8">
+        <v>0</v>
+      </c>
+      <c r="F44" s="8">
+        <v>0</v>
+      </c>
+      <c r="G44" s="8">
         <v>0.4</v>
       </c>
-      <c r="H44" s="9">
+      <c r="H44" s="8">
         <v>2</v>
       </c>
       <c r="I44" s="1" t="s">
@@ -3199,25 +3185,25 @@
       <c r="A45" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="B45" s="9" t="s">
+      <c r="B45" s="8" t="s">
         <v>216</v>
       </c>
-      <c r="C45" s="9">
-        <v>0</v>
-      </c>
-      <c r="D45" s="9">
-        <v>0.2</v>
-      </c>
-      <c r="E45" s="9">
-        <v>0</v>
-      </c>
-      <c r="F45" s="9">
-        <v>0</v>
-      </c>
-      <c r="G45" s="9">
+      <c r="C45" s="8">
+        <v>0</v>
+      </c>
+      <c r="D45" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="E45" s="8">
+        <v>0</v>
+      </c>
+      <c r="F45" s="8">
+        <v>0</v>
+      </c>
+      <c r="G45" s="8">
         <v>0.4</v>
       </c>
-      <c r="H45" s="9">
+      <c r="H45" s="8">
         <v>2</v>
       </c>
       <c r="I45" s="1" t="s">
@@ -3228,25 +3214,25 @@
       <c r="A46" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="B46" s="9" t="s">
+      <c r="B46" s="8" t="s">
         <v>218</v>
       </c>
-      <c r="C46" s="9">
-        <v>0</v>
-      </c>
-      <c r="D46" s="9">
-        <v>0</v>
-      </c>
-      <c r="E46" s="9">
-        <v>0.2</v>
-      </c>
-      <c r="F46" s="9">
-        <v>0</v>
-      </c>
-      <c r="G46" s="9">
+      <c r="C46" s="8">
+        <v>0</v>
+      </c>
+      <c r="D46" s="8">
+        <v>0</v>
+      </c>
+      <c r="E46" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="F46" s="8">
+        <v>0</v>
+      </c>
+      <c r="G46" s="8">
         <v>0.4</v>
       </c>
-      <c r="H46" s="9">
+      <c r="H46" s="8">
         <v>2</v>
       </c>
       <c r="I46" s="1" t="s">
@@ -3257,25 +3243,25 @@
       <c r="A47" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="B47" s="9" t="s">
+      <c r="B47" s="8" t="s">
         <v>220</v>
       </c>
-      <c r="C47" s="9">
-        <v>0</v>
-      </c>
-      <c r="D47" s="9">
-        <v>0</v>
-      </c>
-      <c r="E47" s="9">
-        <v>0</v>
-      </c>
-      <c r="F47" s="9">
-        <v>0.2</v>
-      </c>
-      <c r="G47" s="9">
+      <c r="C47" s="8">
+        <v>0</v>
+      </c>
+      <c r="D47" s="8">
+        <v>0</v>
+      </c>
+      <c r="E47" s="8">
+        <v>0</v>
+      </c>
+      <c r="F47" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="G47" s="8">
         <v>0.4</v>
       </c>
-      <c r="H47" s="9">
+      <c r="H47" s="8">
         <v>2</v>
       </c>
       <c r="I47" s="1" t="s">
@@ -3286,25 +3272,25 @@
       <c r="A48" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="B48" s="9" t="s">
+      <c r="B48" s="8" t="s">
         <v>222</v>
       </c>
-      <c r="C48" s="9">
-        <v>0</v>
-      </c>
-      <c r="D48" s="9">
-        <v>0.2</v>
-      </c>
-      <c r="E48" s="9">
+      <c r="C48" s="8">
+        <v>0</v>
+      </c>
+      <c r="D48" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="E48" s="8">
         <v>0.4</v>
       </c>
-      <c r="F48" s="9">
-        <v>0.2</v>
-      </c>
-      <c r="G48" s="9">
+      <c r="F48" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="G48" s="8">
         <v>0.4</v>
       </c>
-      <c r="H48" s="9">
+      <c r="H48" s="8">
         <v>4</v>
       </c>
       <c r="I48" s="1" t="s">
@@ -3315,25 +3301,25 @@
       <c r="A49" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="B49" s="9" t="s">
+      <c r="B49" s="8" t="s">
         <v>224</v>
       </c>
-      <c r="C49" s="9">
-        <v>0</v>
-      </c>
-      <c r="D49" s="9">
+      <c r="C49" s="8">
+        <v>0</v>
+      </c>
+      <c r="D49" s="8">
         <v>0.4</v>
       </c>
-      <c r="E49" s="9">
-        <v>0.2</v>
-      </c>
-      <c r="F49" s="9">
+      <c r="E49" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="F49" s="8">
         <v>0.4</v>
       </c>
-      <c r="G49" s="9">
-        <v>0.2</v>
-      </c>
-      <c r="H49" s="9">
+      <c r="G49" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="H49" s="8">
         <v>4</v>
       </c>
       <c r="I49" s="1" t="s">
@@ -3344,25 +3330,25 @@
       <c r="A50" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="B50" s="9" t="s">
+      <c r="B50" s="8" t="s">
         <v>226</v>
       </c>
-      <c r="C50" s="9">
-        <v>0</v>
-      </c>
-      <c r="D50" s="9">
+      <c r="C50" s="8">
+        <v>0</v>
+      </c>
+      <c r="D50" s="8">
         <v>0.4</v>
       </c>
-      <c r="E50" s="9">
+      <c r="E50" s="8">
         <v>0.4</v>
       </c>
-      <c r="F50" s="9">
-        <v>0.2</v>
-      </c>
-      <c r="G50" s="9">
-        <v>0.2</v>
-      </c>
-      <c r="H50" s="9">
+      <c r="F50" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="G50" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="H50" s="8">
         <v>4</v>
       </c>
       <c r="I50" s="1" t="s">
@@ -3373,25 +3359,25 @@
       <c r="A51" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="B51" s="9" t="s">
+      <c r="B51" s="8" t="s">
         <v>228</v>
       </c>
-      <c r="C51" s="9">
-        <v>0</v>
-      </c>
-      <c r="D51" s="9">
-        <v>0.2</v>
-      </c>
-      <c r="E51" s="9">
+      <c r="C51" s="8">
+        <v>0</v>
+      </c>
+      <c r="D51" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="E51" s="8">
         <v>0.4</v>
       </c>
-      <c r="F51" s="9">
+      <c r="F51" s="8">
         <v>0.4</v>
       </c>
-      <c r="G51" s="9">
-        <v>0.2</v>
-      </c>
-      <c r="H51" s="9">
+      <c r="G51" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="H51" s="8">
         <v>4</v>
       </c>
       <c r="I51" s="1" t="s">
@@ -3408,191 +3394,4 @@
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCC343D5-ACEC-440C-BE2B-40BCC1E75BAA}">
-  <dimension ref="A1:AB2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="B1" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="E1" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="F1" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="G1" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="H1" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="I1" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="J1" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="K1" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="L1" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="M1" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="N1" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="O1" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="P1" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="Q1" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="R1" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="S1" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="T1" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="U1" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="V1" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="W1" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="X1" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="Y1" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="Z1" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="AA1" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="AB1" s="8" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="2" spans="1:28" s="14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="14">
-        <v>1</v>
-      </c>
-      <c r="B2" s="14">
-        <v>1</v>
-      </c>
-      <c r="C2" s="14">
-        <v>1</v>
-      </c>
-      <c r="D2" s="14">
-        <v>1</v>
-      </c>
-      <c r="E2" s="14">
-        <v>1</v>
-      </c>
-      <c r="F2" s="14">
-        <v>1</v>
-      </c>
-      <c r="G2" s="14">
-        <v>1</v>
-      </c>
-      <c r="H2" s="14">
-        <v>1</v>
-      </c>
-      <c r="I2" s="14">
-        <v>1</v>
-      </c>
-      <c r="J2" s="14">
-        <v>1</v>
-      </c>
-      <c r="K2" s="14">
-        <v>1</v>
-      </c>
-      <c r="L2" s="14">
-        <v>1</v>
-      </c>
-      <c r="M2" s="14">
-        <v>1</v>
-      </c>
-      <c r="N2" s="14">
-        <v>1</v>
-      </c>
-      <c r="O2" s="14">
-        <v>0</v>
-      </c>
-      <c r="P2" s="14">
-        <v>0</v>
-      </c>
-      <c r="Q2" s="14">
-        <v>0</v>
-      </c>
-      <c r="R2" s="14">
-        <v>0</v>
-      </c>
-      <c r="S2" s="14">
-        <v>0</v>
-      </c>
-      <c r="T2" s="14">
-        <v>1</v>
-      </c>
-      <c r="U2" s="14">
-        <v>1</v>
-      </c>
-      <c r="V2" s="14">
-        <v>0</v>
-      </c>
-      <c r="W2" s="14">
-        <v>1</v>
-      </c>
-      <c r="X2" s="14">
-        <v>0</v>
-      </c>
-      <c r="Y2" s="14">
-        <v>1</v>
-      </c>
-      <c r="Z2" s="14">
-        <v>0</v>
-      </c>
-      <c r="AA2" s="14">
-        <v>1</v>
-      </c>
-      <c r="AB2" s="14">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>